<commit_message>
First test: read an Excel File
</commit_message>
<xml_diff>
--- a/MusicDatabase.xlsx
+++ b/MusicDatabase.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/el/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/el/Documents/GitHub/Transcripteur-de-notes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B2A016D-3D3E-4347-AF45-6D7FB02B0BE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDDC6F04-526D-AA4C-90A3-8BCFEF21CD8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3260" yWindow="2160" windowWidth="28040" windowHeight="17440" xr2:uid="{92A7D150-E342-6A40-AE5E-1540E9F29EF8}"/>
+    <workbookView xWindow="6940" yWindow="2220" windowWidth="28040" windowHeight="17440" activeTab="1" xr2:uid="{92A7D150-E342-6A40-AE5E-1540E9F29EF8}"/>
   </bookViews>
   <sheets>
     <sheet name="RAW_DATA" sheetId="1" r:id="rId1"/>
@@ -39,13 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
-  <si>
-    <t>Duration</t>
-  </si>
-  <si>
-    <t>Frequency</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="9">
   <si>
     <t>Tempo</t>
   </si>
@@ -58,12 +52,27 @@
   <si>
     <t>TimeSignature</t>
   </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>Duration(ms)</t>
+  </si>
+  <si>
+    <t>Frequency(Hz)</t>
+  </si>
+  <si>
+    <t>Note</t>
+  </si>
+  <si>
+    <t>Rythmn</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -77,6 +86,11 @@
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF0E0E0E"/>
+      <name val=".SF NS"/>
     </font>
   </fonts>
   <fills count="2">
@@ -99,14 +113,54 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="7">
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color rgb="FF0E0E0E"/>
+        <name val=".SF NS"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -1804,6 +1858,31 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{835927DE-8815-EF46-99F7-0DF9B01410F4}" name="Table1" displayName="Table1" ref="A1:C15" totalsRowShown="0">
+  <autoFilter ref="A1:C15" xr:uid="{835927DE-8815-EF46-99F7-0DF9B01410F4}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{450BF35A-9FCC-1145-8BFE-45939F271A92}" name="IDSong"/>
+    <tableColumn id="2" xr3:uid="{D5EA15CA-0A28-5F48-BB1E-6650B5FB81C2}" name="Duration(ms)"/>
+    <tableColumn id="3" xr3:uid="{82180FAF-280A-B24D-A6B4-8DCA8D912F99}" name="Frequency(Hz)" dataDxfId="6"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{EEC351DF-B4FF-0646-94F1-C310C8DD727D}" name="Table2" displayName="Table2" ref="A1:D2" totalsRowShown="0" headerRowDxfId="1" dataDxfId="0">
+  <autoFilter ref="A1:D2" xr:uid="{EEC351DF-B4FF-0646-94F1-C310C8DD727D}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{E99718A0-1938-684D-BEAA-C3B93C019C29}" name="IDSong" dataDxfId="5"/>
+    <tableColumn id="2" xr3:uid="{A4D5759E-75E7-5745-B428-0C5D8E3708D8}" name="Tempo" dataDxfId="4"/>
+    <tableColumn id="3" xr3:uid="{3AEF52CE-DBA3-8242-B152-38551FF06277}" name="Key" dataDxfId="3"/>
+    <tableColumn id="4" xr3:uid="{2FF6B7FC-9AA9-AD49-8A18-E41A6F579806}" name="TimeSignature" dataDxfId="2"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2123,69 +2202,263 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25138379-DD64-5E40-9BE1-27C8B5E1E507}">
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:C15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L14" sqref="L14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="2" max="2" width="14.6640625" customWidth="1"/>
+    <col min="3" max="3" width="15.5" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="18">
+      <c r="A2">
         <v>1</v>
       </c>
-      <c r="B1" t="s">
-        <v>0</v>
+      <c r="B2">
+        <v>1000</v>
+      </c>
+      <c r="C2" s="2">
+        <v>261.63</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="18">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>1000</v>
+      </c>
+      <c r="C3" s="2">
+        <v>261.63</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="18">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4">
+        <v>1000</v>
+      </c>
+      <c r="C4" s="2">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="18">
+      <c r="A5">
+        <v>1</v>
+      </c>
+      <c r="B5">
+        <v>1000</v>
+      </c>
+      <c r="C5" s="2">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="18">
+      <c r="A6">
+        <v>1</v>
+      </c>
+      <c r="B6">
+        <v>1000</v>
+      </c>
+      <c r="C6" s="2">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="18">
+      <c r="A7">
+        <v>1</v>
+      </c>
+      <c r="B7">
+        <v>1000</v>
+      </c>
+      <c r="C7" s="2">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="18">
+      <c r="A8">
+        <v>1</v>
+      </c>
+      <c r="B8">
+        <v>2000</v>
+      </c>
+      <c r="C8" s="2">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="18">
+      <c r="A9">
+        <v>1</v>
+      </c>
+      <c r="B9">
+        <v>1000</v>
+      </c>
+      <c r="C9" s="2">
+        <v>349.23</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="18">
+      <c r="A10">
+        <v>1</v>
+      </c>
+      <c r="B10">
+        <v>1000</v>
+      </c>
+      <c r="C10" s="2">
+        <v>349.23</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="18">
+      <c r="A11">
+        <v>1</v>
+      </c>
+      <c r="B11">
+        <v>1000</v>
+      </c>
+      <c r="C11" s="2">
+        <v>329.63</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="18">
+      <c r="A12">
+        <v>1</v>
+      </c>
+      <c r="B12">
+        <v>1000</v>
+      </c>
+      <c r="C12" s="2">
+        <v>329.63</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="18">
+      <c r="A13">
+        <v>1</v>
+      </c>
+      <c r="B13">
+        <v>1000</v>
+      </c>
+      <c r="C13" s="2">
+        <v>293.66000000000003</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="18">
+      <c r="A14">
+        <v>1</v>
+      </c>
+      <c r="B14">
+        <v>1000</v>
+      </c>
+      <c r="C14" s="2">
+        <v>293.66000000000003</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="18">
+      <c r="A15">
+        <v>1</v>
+      </c>
+      <c r="B15">
+        <v>2000</v>
+      </c>
+      <c r="C15" s="2">
+        <v>261.63</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19AC43FA-0314-0A45-B9FF-F9BEFE45DA2F}">
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="3" max="3" width="12.83203125" customWidth="1"/>
+    <col min="4" max="4" width="15.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+    <row r="1" spans="1:4">
+      <c r="A1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="3">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3">
+        <v>60</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D1" t="s">
-        <v>5</v>
+      <c r="D2" s="3">
+        <v>4</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48C4D8DE-B7E4-1C4A-B099-79BFF4A8E6AA}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="C1" sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -2198,9 +2471,9 @@
       <selection activeCell="AK54" sqref="AK54"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <sheetData>
-    <row r="4" spans="4:36" ht="20" x14ac:dyDescent="0.25">
+    <row r="4" spans="4:36" ht="20">
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
@@ -2235,7 +2508,7 @@
       <c r="AI4" s="1"/>
       <c r="AJ4" s="1"/>
     </row>
-    <row r="5" spans="4:36" ht="20" x14ac:dyDescent="0.25">
+    <row r="5" spans="4:36" ht="20">
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
@@ -2270,7 +2543,7 @@
       <c r="AI5" s="1"/>
       <c r="AJ5" s="1"/>
     </row>
-    <row r="6" spans="4:36" ht="20" x14ac:dyDescent="0.25">
+    <row r="6" spans="4:36" ht="20">
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
@@ -2305,7 +2578,7 @@
       <c r="AI6" s="1"/>
       <c r="AJ6" s="1"/>
     </row>
-    <row r="7" spans="4:36" ht="20" x14ac:dyDescent="0.25">
+    <row r="7" spans="4:36" ht="20">
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
@@ -2340,7 +2613,7 @@
       <c r="AI7" s="1"/>
       <c r="AJ7" s="1"/>
     </row>
-    <row r="8" spans="4:36" ht="20" x14ac:dyDescent="0.25">
+    <row r="8" spans="4:36" ht="20">
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
@@ -2375,7 +2648,7 @@
       <c r="AI8" s="1"/>
       <c r="AJ8" s="1"/>
     </row>
-    <row r="9" spans="4:36" ht="20" x14ac:dyDescent="0.25">
+    <row r="9" spans="4:36" ht="20">
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
@@ -2410,7 +2683,7 @@
       <c r="AI9" s="1"/>
       <c r="AJ9" s="1"/>
     </row>
-    <row r="10" spans="4:36" ht="20" x14ac:dyDescent="0.25">
+    <row r="10" spans="4:36" ht="20">
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
@@ -2445,7 +2718,7 @@
       <c r="AI10" s="1"/>
       <c r="AJ10" s="1"/>
     </row>
-    <row r="11" spans="4:36" ht="20" x14ac:dyDescent="0.25">
+    <row r="11" spans="4:36" ht="20">
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
@@ -2480,7 +2753,7 @@
       <c r="AI11" s="1"/>
       <c r="AJ11" s="1"/>
     </row>
-    <row r="12" spans="4:36" ht="20" x14ac:dyDescent="0.25">
+    <row r="12" spans="4:36" ht="20">
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
@@ -2515,7 +2788,7 @@
       <c r="AI12" s="1"/>
       <c r="AJ12" s="1"/>
     </row>
-    <row r="13" spans="4:36" ht="20" x14ac:dyDescent="0.25">
+    <row r="13" spans="4:36" ht="20">
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
@@ -2550,7 +2823,7 @@
       <c r="AI13" s="1"/>
       <c r="AJ13" s="1"/>
     </row>
-    <row r="14" spans="4:36" ht="20" x14ac:dyDescent="0.25">
+    <row r="14" spans="4:36" ht="20">
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
@@ -2585,7 +2858,7 @@
       <c r="AI14" s="1"/>
       <c r="AJ14" s="1"/>
     </row>
-    <row r="15" spans="4:36" ht="20" x14ac:dyDescent="0.25">
+    <row r="15" spans="4:36" ht="20">
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
@@ -2620,7 +2893,7 @@
       <c r="AI15" s="1"/>
       <c r="AJ15" s="1"/>
     </row>
-    <row r="16" spans="4:36" ht="20" x14ac:dyDescent="0.25">
+    <row r="16" spans="4:36" ht="20">
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
@@ -2655,7 +2928,7 @@
       <c r="AI16" s="1"/>
       <c r="AJ16" s="1"/>
     </row>
-    <row r="17" spans="4:36" ht="20" x14ac:dyDescent="0.25">
+    <row r="17" spans="4:36" ht="20">
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
@@ -2690,7 +2963,7 @@
       <c r="AI17" s="1"/>
       <c r="AJ17" s="1"/>
     </row>
-    <row r="18" spans="4:36" ht="20" x14ac:dyDescent="0.25">
+    <row r="18" spans="4:36" ht="20">
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>
@@ -2725,7 +2998,7 @@
       <c r="AI18" s="1"/>
       <c r="AJ18" s="1"/>
     </row>
-    <row r="19" spans="4:36" ht="20" x14ac:dyDescent="0.25">
+    <row r="19" spans="4:36" ht="20">
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
       <c r="F19" s="1"/>
@@ -2760,7 +3033,7 @@
       <c r="AI19" s="1"/>
       <c r="AJ19" s="1"/>
     </row>
-    <row r="20" spans="4:36" ht="20" x14ac:dyDescent="0.25">
+    <row r="20" spans="4:36" ht="20">
       <c r="D20" s="1"/>
       <c r="E20" s="1"/>
       <c r="F20" s="1"/>
@@ -2795,7 +3068,7 @@
       <c r="AI20" s="1"/>
       <c r="AJ20" s="1"/>
     </row>
-    <row r="21" spans="4:36" ht="20" x14ac:dyDescent="0.25">
+    <row r="21" spans="4:36" ht="20">
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
       <c r="F21" s="1"/>
@@ -2830,7 +3103,7 @@
       <c r="AI21" s="1"/>
       <c r="AJ21" s="1"/>
     </row>
-    <row r="22" spans="4:36" ht="20" x14ac:dyDescent="0.25">
+    <row r="22" spans="4:36" ht="20">
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>
       <c r="F22" s="1"/>
@@ -2865,7 +3138,7 @@
       <c r="AI22" s="1"/>
       <c r="AJ22" s="1"/>
     </row>
-    <row r="23" spans="4:36" ht="20" x14ac:dyDescent="0.25">
+    <row r="23" spans="4:36" ht="20">
       <c r="D23" s="1"/>
       <c r="E23" s="1"/>
       <c r="F23" s="1"/>
@@ -2900,7 +3173,7 @@
       <c r="AI23" s="1"/>
       <c r="AJ23" s="1"/>
     </row>
-    <row r="24" spans="4:36" ht="20" x14ac:dyDescent="0.25">
+    <row r="24" spans="4:36" ht="20">
       <c r="D24" s="1"/>
       <c r="E24" s="1"/>
       <c r="F24" s="1"/>
@@ -2935,7 +3208,7 @@
       <c r="AI24" s="1"/>
       <c r="AJ24" s="1"/>
     </row>
-    <row r="25" spans="4:36" ht="20" x14ac:dyDescent="0.25">
+    <row r="25" spans="4:36" ht="20">
       <c r="D25" s="1"/>
       <c r="E25" s="1"/>
       <c r="F25" s="1"/>
@@ -2970,7 +3243,7 @@
       <c r="AI25" s="1"/>
       <c r="AJ25" s="1"/>
     </row>
-    <row r="26" spans="4:36" ht="20" x14ac:dyDescent="0.25">
+    <row r="26" spans="4:36" ht="20">
       <c r="D26" s="1"/>
       <c r="E26" s="1"/>
       <c r="F26" s="1"/>
@@ -3005,7 +3278,7 @@
       <c r="AI26" s="1"/>
       <c r="AJ26" s="1"/>
     </row>
-    <row r="27" spans="4:36" ht="20" x14ac:dyDescent="0.25">
+    <row r="27" spans="4:36" ht="20">
       <c r="D27" s="1"/>
       <c r="E27" s="1"/>
       <c r="F27" s="1"/>
@@ -3040,7 +3313,7 @@
       <c r="AI27" s="1"/>
       <c r="AJ27" s="1"/>
     </row>
-    <row r="28" spans="4:36" ht="20" x14ac:dyDescent="0.25">
+    <row r="28" spans="4:36" ht="20">
       <c r="D28" s="1"/>
       <c r="E28" s="1"/>
       <c r="F28" s="1"/>
@@ -3075,7 +3348,7 @@
       <c r="AI28" s="1"/>
       <c r="AJ28" s="1"/>
     </row>
-    <row r="29" spans="4:36" ht="20" x14ac:dyDescent="0.25">
+    <row r="29" spans="4:36" ht="20">
       <c r="D29" s="1"/>
       <c r="E29" s="1"/>
       <c r="F29" s="1"/>
@@ -3110,7 +3383,7 @@
       <c r="AI29" s="1"/>
       <c r="AJ29" s="1"/>
     </row>
-    <row r="30" spans="4:36" ht="20" x14ac:dyDescent="0.25">
+    <row r="30" spans="4:36" ht="20">
       <c r="D30" s="1"/>
       <c r="E30" s="1"/>
       <c r="F30" s="1"/>
@@ -3145,7 +3418,7 @@
       <c r="AI30" s="1"/>
       <c r="AJ30" s="1"/>
     </row>
-    <row r="31" spans="4:36" ht="20" x14ac:dyDescent="0.25">
+    <row r="31" spans="4:36" ht="20">
       <c r="D31" s="1"/>
       <c r="E31" s="1"/>
       <c r="F31" s="1"/>
@@ -3180,7 +3453,7 @@
       <c r="AI31" s="1"/>
       <c r="AJ31" s="1"/>
     </row>
-    <row r="32" spans="4:36" ht="20" x14ac:dyDescent="0.25">
+    <row r="32" spans="4:36" ht="20">
       <c r="D32" s="1"/>
       <c r="E32" s="1"/>
       <c r="F32" s="1"/>
@@ -3215,7 +3488,7 @@
       <c r="AI32" s="1"/>
       <c r="AJ32" s="1"/>
     </row>
-    <row r="33" spans="4:36" ht="20" x14ac:dyDescent="0.25">
+    <row r="33" spans="4:36" ht="20">
       <c r="D33" s="1"/>
       <c r="E33" s="1"/>
       <c r="F33" s="1"/>
@@ -3250,7 +3523,7 @@
       <c r="AI33" s="1"/>
       <c r="AJ33" s="1"/>
     </row>
-    <row r="34" spans="4:36" ht="20" x14ac:dyDescent="0.25">
+    <row r="34" spans="4:36" ht="20">
       <c r="D34" s="1"/>
       <c r="E34" s="1"/>
       <c r="F34" s="1"/>
@@ -3285,7 +3558,7 @@
       <c r="AI34" s="1"/>
       <c r="AJ34" s="1"/>
     </row>
-    <row r="35" spans="4:36" ht="20" x14ac:dyDescent="0.25">
+    <row r="35" spans="4:36" ht="20">
       <c r="D35" s="1"/>
       <c r="E35" s="1"/>
       <c r="F35" s="1"/>
@@ -3320,7 +3593,7 @@
       <c r="AI35" s="1"/>
       <c r="AJ35" s="1"/>
     </row>
-    <row r="36" spans="4:36" ht="20" x14ac:dyDescent="0.25">
+    <row r="36" spans="4:36" ht="20">
       <c r="D36" s="1"/>
       <c r="E36" s="1"/>
       <c r="F36" s="1"/>
@@ -3355,7 +3628,7 @@
       <c r="AI36" s="1"/>
       <c r="AJ36" s="1"/>
     </row>
-    <row r="37" spans="4:36" ht="20" x14ac:dyDescent="0.25">
+    <row r="37" spans="4:36" ht="20">
       <c r="D37" s="1"/>
       <c r="E37" s="1"/>
       <c r="F37" s="1"/>
@@ -3390,7 +3663,7 @@
       <c r="AI37" s="1"/>
       <c r="AJ37" s="1"/>
     </row>
-    <row r="38" spans="4:36" ht="20" x14ac:dyDescent="0.25">
+    <row r="38" spans="4:36" ht="20">
       <c r="D38" s="1"/>
       <c r="E38" s="1"/>
       <c r="F38" s="1"/>
@@ -3425,7 +3698,7 @@
       <c r="AI38" s="1"/>
       <c r="AJ38" s="1"/>
     </row>
-    <row r="39" spans="4:36" ht="20" x14ac:dyDescent="0.25">
+    <row r="39" spans="4:36" ht="20">
       <c r="D39" s="1"/>
       <c r="E39" s="1"/>
       <c r="F39" s="1"/>
@@ -3460,7 +3733,7 @@
       <c r="AI39" s="1"/>
       <c r="AJ39" s="1"/>
     </row>
-    <row r="40" spans="4:36" ht="20" x14ac:dyDescent="0.25">
+    <row r="40" spans="4:36" ht="20">
       <c r="D40" s="1"/>
       <c r="E40" s="1"/>
       <c r="F40" s="1"/>
@@ -3495,7 +3768,7 @@
       <c r="AI40" s="1"/>
       <c r="AJ40" s="1"/>
     </row>
-    <row r="41" spans="4:36" ht="20" x14ac:dyDescent="0.25">
+    <row r="41" spans="4:36" ht="20">
       <c r="D41" s="1"/>
       <c r="E41" s="1"/>
       <c r="F41" s="1"/>
@@ -3530,7 +3803,7 @@
       <c r="AI41" s="1"/>
       <c r="AJ41" s="1"/>
     </row>
-    <row r="42" spans="4:36" ht="20" x14ac:dyDescent="0.25">
+    <row r="42" spans="4:36" ht="20">
       <c r="D42" s="1"/>
       <c r="E42" s="1"/>
       <c r="F42" s="1"/>
@@ -3565,7 +3838,7 @@
       <c r="AI42" s="1"/>
       <c r="AJ42" s="1"/>
     </row>
-    <row r="43" spans="4:36" ht="20" x14ac:dyDescent="0.25">
+    <row r="43" spans="4:36" ht="20">
       <c r="D43" s="1"/>
       <c r="E43" s="1"/>
       <c r="F43" s="1"/>
@@ -3600,7 +3873,7 @@
       <c r="AI43" s="1"/>
       <c r="AJ43" s="1"/>
     </row>
-    <row r="44" spans="4:36" ht="20" x14ac:dyDescent="0.25">
+    <row r="44" spans="4:36" ht="20">
       <c r="D44" s="1"/>
       <c r="E44" s="1"/>
       <c r="F44" s="1"/>
@@ -3635,7 +3908,7 @@
       <c r="AI44" s="1"/>
       <c r="AJ44" s="1"/>
     </row>
-    <row r="45" spans="4:36" ht="20" x14ac:dyDescent="0.25">
+    <row r="45" spans="4:36" ht="20">
       <c r="D45" s="1"/>
       <c r="E45" s="1"/>
       <c r="F45" s="1"/>
@@ -3670,7 +3943,7 @@
       <c r="AI45" s="1"/>
       <c r="AJ45" s="1"/>
     </row>
-    <row r="46" spans="4:36" ht="20" x14ac:dyDescent="0.25">
+    <row r="46" spans="4:36" ht="20">
       <c r="D46" s="1"/>
       <c r="E46" s="1"/>
       <c r="F46" s="1"/>
@@ -3705,7 +3978,7 @@
       <c r="AI46" s="1"/>
       <c r="AJ46" s="1"/>
     </row>
-    <row r="47" spans="4:36" ht="20" x14ac:dyDescent="0.25">
+    <row r="47" spans="4:36" ht="20">
       <c r="D47" s="1"/>
       <c r="E47" s="1"/>
       <c r="F47" s="1"/>
@@ -3740,7 +4013,7 @@
       <c r="AI47" s="1"/>
       <c r="AJ47" s="1"/>
     </row>
-    <row r="48" spans="4:36" ht="20" x14ac:dyDescent="0.25">
+    <row r="48" spans="4:36" ht="20">
       <c r="D48" s="1"/>
       <c r="E48" s="1"/>
       <c r="F48" s="1"/>
@@ -3775,7 +4048,7 @@
       <c r="AI48" s="1"/>
       <c r="AJ48" s="1"/>
     </row>
-    <row r="49" spans="4:36" ht="20" x14ac:dyDescent="0.25">
+    <row r="49" spans="4:36" ht="20">
       <c r="D49" s="1"/>
       <c r="E49" s="1"/>
       <c r="F49" s="1"/>
@@ -3810,7 +4083,7 @@
       <c r="AI49" s="1"/>
       <c r="AJ49" s="1"/>
     </row>
-    <row r="50" spans="4:36" ht="20" x14ac:dyDescent="0.25">
+    <row r="50" spans="4:36" ht="20">
       <c r="D50" s="1"/>
       <c r="E50" s="1"/>
       <c r="F50" s="1"/>
@@ -3845,7 +4118,7 @@
       <c r="AI50" s="1"/>
       <c r="AJ50" s="1"/>
     </row>
-    <row r="51" spans="4:36" ht="20" x14ac:dyDescent="0.25">
+    <row r="51" spans="4:36" ht="20">
       <c r="D51" s="1"/>
       <c r="E51" s="1"/>
       <c r="F51" s="1"/>
@@ -3880,7 +4153,7 @@
       <c r="AI51" s="1"/>
       <c r="AJ51" s="1"/>
     </row>
-    <row r="52" spans="4:36" ht="20" x14ac:dyDescent="0.25">
+    <row r="52" spans="4:36" ht="20">
       <c r="D52" s="1"/>
       <c r="E52" s="1"/>
       <c r="F52" s="1"/>
@@ -3914,7 +4187,7 @@
       <c r="AI52" s="1"/>
       <c r="AJ52" s="1"/>
     </row>
-    <row r="53" spans="4:36" ht="20" x14ac:dyDescent="0.25">
+    <row r="53" spans="4:36" ht="20">
       <c r="D53" s="1"/>
       <c r="E53" s="1"/>
       <c r="F53" s="1"/>
@@ -3948,7 +4221,7 @@
       <c r="AI53" s="1"/>
       <c r="AJ53" s="1"/>
     </row>
-    <row r="54" spans="4:36" ht="20" x14ac:dyDescent="0.25">
+    <row r="54" spans="4:36" ht="20">
       <c r="D54" s="1"/>
       <c r="E54" s="1"/>
       <c r="F54" s="1"/>
@@ -3982,7 +4255,7 @@
       <c r="AI54" s="1"/>
       <c r="AJ54" s="1"/>
     </row>
-    <row r="55" spans="4:36" ht="20" x14ac:dyDescent="0.25">
+    <row r="55" spans="4:36" ht="20">
       <c r="D55" s="1"/>
       <c r="E55" s="1"/>
       <c r="F55" s="1"/>
@@ -4016,7 +4289,7 @@
       <c r="AI55" s="1"/>
       <c r="AJ55" s="1"/>
     </row>
-    <row r="56" spans="4:36" ht="20" x14ac:dyDescent="0.25">
+    <row r="56" spans="4:36" ht="20">
       <c r="D56" s="1"/>
       <c r="E56" s="1"/>
       <c r="F56" s="1"/>
@@ -4050,7 +4323,7 @@
       <c r="AI56" s="1"/>
       <c r="AJ56" s="1"/>
     </row>
-    <row r="57" spans="4:36" ht="20" x14ac:dyDescent="0.25">
+    <row r="57" spans="4:36" ht="20">
       <c r="D57" s="1"/>
       <c r="E57" s="1"/>
       <c r="F57" s="1"/>
@@ -4084,7 +4357,7 @@
       <c r="AI57" s="1"/>
       <c r="AJ57" s="1"/>
     </row>
-    <row r="58" spans="4:36" ht="20" x14ac:dyDescent="0.25">
+    <row r="58" spans="4:36" ht="20">
       <c r="D58" s="1"/>
       <c r="E58" s="1"/>
       <c r="F58" s="1"/>
@@ -4118,7 +4391,7 @@
       <c r="AI58" s="1"/>
       <c r="AJ58" s="1"/>
     </row>
-    <row r="59" spans="4:36" ht="20" x14ac:dyDescent="0.25">
+    <row r="59" spans="4:36" ht="20">
       <c r="D59" s="1"/>
       <c r="E59" s="1"/>
       <c r="F59" s="1"/>
@@ -4152,7 +4425,7 @@
       <c r="AI59" s="1"/>
       <c r="AJ59" s="1"/>
     </row>
-    <row r="60" spans="4:36" ht="20" x14ac:dyDescent="0.25">
+    <row r="60" spans="4:36" ht="20">
       <c r="D60" s="1"/>
       <c r="E60" s="1"/>
       <c r="F60" s="1"/>
@@ -4186,7 +4459,7 @@
       <c r="AI60" s="1"/>
       <c r="AJ60" s="1"/>
     </row>
-    <row r="61" spans="4:36" ht="20" x14ac:dyDescent="0.25">
+    <row r="61" spans="4:36" ht="20">
       <c r="D61" s="1"/>
       <c r="E61" s="1"/>
       <c r="F61" s="1"/>
@@ -4220,7 +4493,7 @@
       <c r="AI61" s="1"/>
       <c r="AJ61" s="1"/>
     </row>
-    <row r="62" spans="4:36" ht="20" x14ac:dyDescent="0.25">
+    <row r="62" spans="4:36" ht="20">
       <c r="D62" s="1"/>
       <c r="E62" s="1"/>
       <c r="F62" s="1"/>
@@ -4254,7 +4527,7 @@
       <c r="AI62" s="1"/>
       <c r="AJ62" s="1"/>
     </row>
-    <row r="63" spans="4:36" ht="20" x14ac:dyDescent="0.25">
+    <row r="63" spans="4:36" ht="20">
       <c r="D63" s="1"/>
       <c r="E63" s="1"/>
       <c r="F63" s="1"/>
@@ -4288,7 +4561,7 @@
       <c r="AI63" s="1"/>
       <c r="AJ63" s="1"/>
     </row>
-    <row r="64" spans="4:36" ht="20" x14ac:dyDescent="0.25">
+    <row r="64" spans="4:36" ht="20">
       <c r="D64" s="1"/>
       <c r="E64" s="1"/>
       <c r="F64" s="1"/>
@@ -4322,7 +4595,7 @@
       <c r="AI64" s="1"/>
       <c r="AJ64" s="1"/>
     </row>
-    <row r="65" spans="4:36" ht="20" x14ac:dyDescent="0.25">
+    <row r="65" spans="4:36" ht="20">
       <c r="D65" s="1"/>
       <c r="E65" s="1"/>
       <c r="F65" s="1"/>
@@ -4356,7 +4629,7 @@
       <c r="AI65" s="1"/>
       <c r="AJ65" s="1"/>
     </row>
-    <row r="66" spans="4:36" ht="20" x14ac:dyDescent="0.25">
+    <row r="66" spans="4:36" ht="20">
       <c r="D66" s="1"/>
       <c r="E66" s="1"/>
       <c r="F66" s="1"/>
@@ -4390,7 +4663,7 @@
       <c r="AI66" s="1"/>
       <c r="AJ66" s="1"/>
     </row>
-    <row r="67" spans="4:36" ht="20" x14ac:dyDescent="0.25">
+    <row r="67" spans="4:36" ht="20">
       <c r="D67" s="1"/>
       <c r="E67" s="1"/>
       <c r="F67" s="1"/>
@@ -4424,7 +4697,7 @@
       <c r="AI67" s="1"/>
       <c r="AJ67" s="1"/>
     </row>
-    <row r="68" spans="4:36" ht="20" x14ac:dyDescent="0.25">
+    <row r="68" spans="4:36" ht="20">
       <c r="D68" s="1"/>
       <c r="E68" s="1"/>
       <c r="F68" s="1"/>
@@ -4458,7 +4731,7 @@
       <c r="AI68" s="1"/>
       <c r="AJ68" s="1"/>
     </row>
-    <row r="69" spans="4:36" ht="20" x14ac:dyDescent="0.25">
+    <row r="69" spans="4:36" ht="20">
       <c r="D69" s="1"/>
       <c r="E69" s="1"/>
       <c r="F69" s="1"/>
@@ -4492,7 +4765,7 @@
       <c r="AI69" s="1"/>
       <c r="AJ69" s="1"/>
     </row>
-    <row r="70" spans="4:36" ht="20" x14ac:dyDescent="0.25">
+    <row r="70" spans="4:36" ht="20">
       <c r="D70" s="1"/>
       <c r="E70" s="1"/>
       <c r="F70" s="1"/>
@@ -4516,7 +4789,7 @@
       <c r="AI70" s="1"/>
       <c r="AJ70" s="1"/>
     </row>
-    <row r="71" spans="4:36" ht="20" x14ac:dyDescent="0.25">
+    <row r="71" spans="4:36" ht="20">
       <c r="D71" s="1"/>
       <c r="E71" s="1"/>
       <c r="F71" s="1"/>
@@ -4540,7 +4813,7 @@
       <c r="AI71" s="1"/>
       <c r="AJ71" s="1"/>
     </row>
-    <row r="72" spans="4:36" ht="20" x14ac:dyDescent="0.25">
+    <row r="72" spans="4:36" ht="20">
       <c r="D72" s="1"/>
       <c r="E72" s="1"/>
       <c r="F72" s="1"/>
@@ -4564,7 +4837,7 @@
       <c r="AI72" s="1"/>
       <c r="AJ72" s="1"/>
     </row>
-    <row r="73" spans="4:36" ht="20" x14ac:dyDescent="0.25">
+    <row r="73" spans="4:36" ht="20">
       <c r="D73" s="1"/>
       <c r="E73" s="1"/>
       <c r="F73" s="1"/>
@@ -4588,7 +4861,7 @@
       <c r="AI73" s="1"/>
       <c r="AJ73" s="1"/>
     </row>
-    <row r="74" spans="4:36" ht="20" x14ac:dyDescent="0.25">
+    <row r="74" spans="4:36" ht="20">
       <c r="D74" s="1"/>
       <c r="E74" s="1"/>
       <c r="F74" s="1"/>
@@ -4612,7 +4885,7 @@
       <c r="AI74" s="1"/>
       <c r="AJ74" s="1"/>
     </row>
-    <row r="75" spans="4:36" ht="20" x14ac:dyDescent="0.25">
+    <row r="75" spans="4:36" ht="20">
       <c r="D75" s="1"/>
       <c r="E75" s="1"/>
       <c r="F75" s="1"/>
@@ -4636,7 +4909,7 @@
       <c r="AI75" s="1"/>
       <c r="AJ75" s="1"/>
     </row>
-    <row r="76" spans="4:36" ht="20" x14ac:dyDescent="0.25">
+    <row r="76" spans="4:36" ht="20">
       <c r="D76" s="1"/>
       <c r="E76" s="1"/>
       <c r="F76" s="1"/>
@@ -4671,7 +4944,7 @@
       <c r="AI76" s="1"/>
       <c r="AJ76" s="1"/>
     </row>
-    <row r="77" spans="4:36" ht="20" x14ac:dyDescent="0.25">
+    <row r="77" spans="4:36" ht="20">
       <c r="D77" s="1"/>
       <c r="E77" s="1"/>
       <c r="F77" s="1"/>

</xml_diff>

<commit_message>
Added Main Functionalities (Data Analysis)
</commit_message>
<xml_diff>
--- a/MusicDatabase.xlsx
+++ b/MusicDatabase.xlsx
@@ -2,52 +2,43 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10916"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/el/Documents/GitHub/Transcripteur-de-notes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDDC6F04-526D-AA4C-90A3-8BCFEF21CD8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{663879F0-66AA-684D-8C1F-8309F9E2B97D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6940" yWindow="2220" windowWidth="28040" windowHeight="17440" activeTab="1" xr2:uid="{92A7D150-E342-6A40-AE5E-1540E9F29EF8}"/>
+    <workbookView xWindow="6940" yWindow="2220" windowWidth="28040" windowHeight="17440" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RAW_DATA" sheetId="1" r:id="rId1"/>
-    <sheet name="REFERENCE" sheetId="3" r:id="rId2"/>
-    <sheet name="PROCESSED_DATA" sheetId="2" r:id="rId3"/>
+    <sheet name="REFERENCE" sheetId="2" r:id="rId2"/>
+    <sheet name="PROCESSED_DATA" sheetId="3" r:id="rId3"/>
     <sheet name="Brainstorming" sheetId="4" r:id="rId4"/>
+    <sheet name="Concept" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="181029"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="18">
+  <si>
+    <t>IdSong</t>
+  </si>
+  <si>
+    <t>Duration(ms)</t>
+  </si>
+  <si>
+    <t>Frequency(Hz)</t>
+  </si>
   <si>
     <t>Tempo</t>
   </si>
   <si>
     <t>Key</t>
-  </si>
-  <si>
-    <t>IDSong</t>
   </si>
   <si>
     <t>TimeSignature</t>
@@ -56,10 +47,7 @@
     <t>C</t>
   </si>
   <si>
-    <t>Duration(ms)</t>
-  </si>
-  <si>
-    <t>Frequency(Hz)</t>
+    <t>4/4</t>
   </si>
   <si>
     <t>Note</t>
@@ -67,12 +55,36 @@
   <si>
     <t>Rythmn</t>
   </si>
+  <si>
+    <t>Quarter Note</t>
+  </si>
+  <si>
+    <t>G</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>Half Note</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>Decibel(db)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -92,6 +104,11 @@
       <color rgb="FF0E0E0E"/>
       <name val=".SF NS"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <name val="Aptos Narrow"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -101,7 +118,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -109,16 +126,37 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -126,38 +164,35 @@
   </cellStyles>
   <dxfs count="7">
     <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="center" vertical="center"/>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center"/>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center"/>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center"/>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center"/>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center"/>
     </dxf>
     <dxf>
       <font>
-        <b val="0"/>
-        <i val="0"/>
         <strike val="0"/>
         <condense val="0"/>
         <extend val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
-        <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="14"/>
         <color rgb="FF0E0E0E"/>
         <name val=".SF NS"/>
-        <scheme val="none"/>
       </font>
     </dxf>
   </dxfs>
@@ -177,13 +212,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>14</xdr:col>
+      <xdr:col>12</xdr:col>
       <xdr:colOff>609600</xdr:colOff>
       <xdr:row>4</xdr:row>
       <xdr:rowOff>190692</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>33</xdr:col>
+      <xdr:col>31</xdr:col>
       <xdr:colOff>304992</xdr:colOff>
       <xdr:row>41</xdr:row>
       <xdr:rowOff>33867</xdr:rowOff>
@@ -193,7 +228,7 @@
         <xdr:cNvPr id="2" name="Rectangle 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{507E9D09-D303-9A49-B7BF-AD2BFD86C488}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D92A2DFC-6FA4-0A47-B41C-CAC08FFF926D}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -238,13 +273,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
+      <xdr:col>1</xdr:col>
       <xdr:colOff>503767</xdr:colOff>
       <xdr:row>4</xdr:row>
       <xdr:rowOff>110066</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
+      <xdr:col>11</xdr:col>
       <xdr:colOff>397934</xdr:colOff>
       <xdr:row>28</xdr:row>
       <xdr:rowOff>135466</xdr:rowOff>
@@ -254,7 +289,7 @@
         <xdr:cNvPr id="3" name="Rectangle 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{21C8FE14-8457-344D-8090-3FF769E7BB4D}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1173F002-5925-FD47-9CE3-6CE727F4D9FA}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -299,13 +334,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
+      <xdr:col>2</xdr:col>
       <xdr:colOff>745067</xdr:colOff>
       <xdr:row>8</xdr:row>
       <xdr:rowOff>156633</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
+      <xdr:col>6</xdr:col>
       <xdr:colOff>59267</xdr:colOff>
       <xdr:row>13</xdr:row>
       <xdr:rowOff>143933</xdr:rowOff>
@@ -315,7 +350,7 @@
         <xdr:cNvPr id="4" name="Rectangle 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C5E8FE24-6996-AC4F-9772-782EA611CD75}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{39132E59-62D0-9041-8B87-FBF472482C9F}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -370,13 +405,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
+      <xdr:col>2</xdr:col>
       <xdr:colOff>812799</xdr:colOff>
       <xdr:row>19</xdr:row>
       <xdr:rowOff>203199</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
+      <xdr:col>6</xdr:col>
       <xdr:colOff>126999</xdr:colOff>
       <xdr:row>24</xdr:row>
       <xdr:rowOff>190499</xdr:rowOff>
@@ -386,7 +421,7 @@
         <xdr:cNvPr id="5" name="Rectangle 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FBB32032-A882-6A42-B5F1-C5165595FDD7}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{69B72ED9-887F-104D-8AAA-B329B5FE4338}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -441,13 +476,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
+      <xdr:col>7</xdr:col>
       <xdr:colOff>673100</xdr:colOff>
       <xdr:row>8</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
+      <xdr:col>10</xdr:col>
       <xdr:colOff>795867</xdr:colOff>
       <xdr:row>17</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -457,7 +492,7 @@
         <xdr:cNvPr id="6" name="Rectangle 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C71EA6E1-9D41-A140-BBD5-854DD16782FD}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{611B5EA4-5CB7-984B-B4F5-52D9CF32273A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -525,13 +560,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>16</xdr:col>
+      <xdr:col>14</xdr:col>
       <xdr:colOff>804562</xdr:colOff>
       <xdr:row>12</xdr:row>
       <xdr:rowOff>67962</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>20</xdr:col>
+      <xdr:col>18</xdr:col>
       <xdr:colOff>68648</xdr:colOff>
       <xdr:row>22</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -541,7 +576,7 @@
         <xdr:cNvPr id="7" name="Rectangle 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{817B9A5F-605B-4F4C-B401-1776C07A4FBB}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B76C2F65-85A3-5E41-9832-E3981239563C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -621,13 +656,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
+      <xdr:col>6</xdr:col>
       <xdr:colOff>59267</xdr:colOff>
       <xdr:row>11</xdr:row>
       <xdr:rowOff>23283</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
+      <xdr:col>7</xdr:col>
       <xdr:colOff>673100</xdr:colOff>
       <xdr:row>12</xdr:row>
       <xdr:rowOff>146050</xdr:rowOff>
@@ -637,7 +672,7 @@
         <xdr:cNvPr id="8" name="Straight Arrow Connector 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B46B0C7F-8519-E842-A604-A1301DE17BD8}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FCAE3095-EDBF-0C40-AC7C-23C688A84F08}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -678,13 +713,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>12</xdr:col>
+      <xdr:col>10</xdr:col>
       <xdr:colOff>795867</xdr:colOff>
       <xdr:row>12</xdr:row>
       <xdr:rowOff>146050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
+      <xdr:col>14</xdr:col>
       <xdr:colOff>804562</xdr:colOff>
       <xdr:row>17</xdr:row>
       <xdr:rowOff>33981</xdr:rowOff>
@@ -694,7 +729,7 @@
         <xdr:cNvPr id="9" name="Straight Arrow Connector 8">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00985B02-6B7E-4C46-9FF2-4ED02A684FE8}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{407B8718-76D0-F449-8BC8-740F8719EEED}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -735,13 +770,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>20</xdr:col>
+      <xdr:col>18</xdr:col>
       <xdr:colOff>68648</xdr:colOff>
       <xdr:row>17</xdr:row>
       <xdr:rowOff>33981</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>22</xdr:col>
+      <xdr:col>20</xdr:col>
       <xdr:colOff>96853</xdr:colOff>
       <xdr:row>17</xdr:row>
       <xdr:rowOff>39224</xdr:rowOff>
@@ -751,7 +786,7 @@
         <xdr:cNvPr id="10" name="Straight Arrow Connector 9">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{16D09642-68DD-A148-9B4A-E1D34D69A942}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4AE31FE2-B096-464E-90C3-95023C45FF80}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -791,13 +826,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>22</xdr:col>
+      <xdr:col>20</xdr:col>
       <xdr:colOff>96853</xdr:colOff>
       <xdr:row>11</xdr:row>
       <xdr:rowOff>78446</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>25</xdr:col>
+      <xdr:col>23</xdr:col>
       <xdr:colOff>398767</xdr:colOff>
       <xdr:row>23</xdr:row>
       <xdr:rowOff>1</xdr:rowOff>
@@ -807,7 +842,7 @@
         <xdr:cNvPr id="11" name="Rectangle 10">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8E437653-6B4B-6244-ACFD-70D36F41391B}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5F0D7E80-9FA6-F943-B364-686EB00431FF}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -914,13 +949,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>27</xdr:col>
+      <xdr:col>25</xdr:col>
       <xdr:colOff>38677</xdr:colOff>
       <xdr:row>17</xdr:row>
       <xdr:rowOff>110258</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>30</xdr:col>
+      <xdr:col>28</xdr:col>
       <xdr:colOff>711777</xdr:colOff>
       <xdr:row>24</xdr:row>
       <xdr:rowOff>115454</xdr:rowOff>
@@ -930,7 +965,7 @@
         <xdr:cNvPr id="12" name="Rectangle 11">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{525D5915-4777-3546-81A5-1EEA8396396E}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{459D97BD-AAE0-4D4D-8D34-32C73D6747AB}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1024,13 +1059,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>22</xdr:col>
+      <xdr:col>20</xdr:col>
       <xdr:colOff>14431</xdr:colOff>
       <xdr:row>32</xdr:row>
       <xdr:rowOff>115454</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>25</xdr:col>
+      <xdr:col>23</xdr:col>
       <xdr:colOff>606136</xdr:colOff>
       <xdr:row>40</xdr:row>
       <xdr:rowOff>72159</xdr:rowOff>
@@ -1040,7 +1075,7 @@
         <xdr:cNvPr id="13" name="Rectangle 12">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{96F1D51B-BA1B-2645-A8D7-44DAB282E649}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{81638593-153D-4A46-9CF2-F44CD556690A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1145,13 +1180,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>27</xdr:col>
+      <xdr:col>25</xdr:col>
       <xdr:colOff>14432</xdr:colOff>
       <xdr:row>24</xdr:row>
       <xdr:rowOff>115454</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>30</xdr:col>
+      <xdr:col>28</xdr:col>
       <xdr:colOff>721591</xdr:colOff>
       <xdr:row>33</xdr:row>
       <xdr:rowOff>101022</xdr:rowOff>
@@ -1161,7 +1196,7 @@
         <xdr:cNvPr id="14" name="Rectangle 13">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3F81E0A7-4C7B-B046-9D42-2B1692DDAFAF}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C65C647B-737F-694B-9FE9-94086C1C4D56}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1227,13 +1262,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>25</xdr:col>
+      <xdr:col>23</xdr:col>
       <xdr:colOff>398767</xdr:colOff>
       <xdr:row>17</xdr:row>
       <xdr:rowOff>39224</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>27</xdr:col>
+      <xdr:col>25</xdr:col>
       <xdr:colOff>38677</xdr:colOff>
       <xdr:row>20</xdr:row>
       <xdr:rowOff>235400</xdr:rowOff>
@@ -1243,7 +1278,7 @@
         <xdr:cNvPr id="15" name="Straight Arrow Connector 14">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CCC92CB3-0711-4841-9421-F688D417632E}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6CCF7D38-4C5D-7348-9988-C3603464EEE3}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1283,13 +1318,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>23</xdr:col>
+      <xdr:col>21</xdr:col>
       <xdr:colOff>721590</xdr:colOff>
       <xdr:row>21</xdr:row>
       <xdr:rowOff>11833</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>27</xdr:col>
+      <xdr:col>25</xdr:col>
       <xdr:colOff>38677</xdr:colOff>
       <xdr:row>32</xdr:row>
       <xdr:rowOff>115454</xdr:rowOff>
@@ -1299,7 +1334,7 @@
         <xdr:cNvPr id="16" name="Straight Arrow Connector 15">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AFEE68CF-6C30-E64F-B709-4A61FE0BB2F1}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{51B4B78F-374B-9F4D-A8AA-6641EDF34AC3}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1339,13 +1374,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>23</xdr:col>
+      <xdr:col>21</xdr:col>
       <xdr:colOff>721590</xdr:colOff>
       <xdr:row>29</xdr:row>
       <xdr:rowOff>7216</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>27</xdr:col>
+      <xdr:col>25</xdr:col>
       <xdr:colOff>14432</xdr:colOff>
       <xdr:row>32</xdr:row>
       <xdr:rowOff>115454</xdr:rowOff>
@@ -1355,7 +1390,7 @@
         <xdr:cNvPr id="17" name="Straight Arrow Connector 16">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E72A842B-75D7-3F4F-9777-4DC07BC9CC77}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{18B84AB6-1EBC-CE48-8C47-F311E7EF0DD1}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1395,13 +1430,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>14</xdr:col>
+      <xdr:col>12</xdr:col>
       <xdr:colOff>643468</xdr:colOff>
       <xdr:row>45</xdr:row>
       <xdr:rowOff>16933</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>23</xdr:col>
+      <xdr:col>21</xdr:col>
       <xdr:colOff>474134</xdr:colOff>
       <xdr:row>66</xdr:row>
       <xdr:rowOff>67733</xdr:rowOff>
@@ -1411,7 +1446,7 @@
         <xdr:cNvPr id="18" name="Rectangle 17">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{81B48673-38B2-B949-B32C-ED5FBFF31F4F}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3C420C37-A51B-C443-9766-1A47E49195A0}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1464,13 +1499,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
+      <xdr:col>5</xdr:col>
       <xdr:colOff>220132</xdr:colOff>
       <xdr:row>5</xdr:row>
       <xdr:rowOff>16933</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
+      <xdr:col>8</xdr:col>
       <xdr:colOff>406400</xdr:colOff>
       <xdr:row>7</xdr:row>
       <xdr:rowOff>50799</xdr:rowOff>
@@ -1480,7 +1515,7 @@
         <xdr:cNvPr id="19" name="TextBox 18">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B6C7AB14-DB68-724B-BF4C-ABE217625E23}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00C00E5F-B58C-4045-BCC7-228DF83AF9D6}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1534,13 +1569,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>24</xdr:col>
+      <xdr:col>22</xdr:col>
       <xdr:colOff>287865</xdr:colOff>
       <xdr:row>5</xdr:row>
       <xdr:rowOff>220132</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>28</xdr:col>
+      <xdr:col>26</xdr:col>
       <xdr:colOff>355600</xdr:colOff>
       <xdr:row>7</xdr:row>
       <xdr:rowOff>203199</xdr:rowOff>
@@ -1550,7 +1585,7 @@
         <xdr:cNvPr id="20" name="TextBox 19">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B246FEDB-BD16-F94C-920F-F0FB059972B7}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E110F24B-1F05-D94F-8BFF-ECCCB332D789}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1609,13 +1644,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>17</xdr:col>
+      <xdr:col>15</xdr:col>
       <xdr:colOff>609600</xdr:colOff>
       <xdr:row>47</xdr:row>
       <xdr:rowOff>101600</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>21</xdr:col>
+      <xdr:col>19</xdr:col>
       <xdr:colOff>457200</xdr:colOff>
       <xdr:row>49</xdr:row>
       <xdr:rowOff>186266</xdr:rowOff>
@@ -1625,7 +1660,7 @@
         <xdr:cNvPr id="21" name="TextBox 20">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6323290A-D6AD-E14D-9969-216E442B2B8D}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{81C7EB56-7A07-9F42-82EA-7894AAD6F0A4}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1679,13 +1714,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>17</xdr:col>
+      <xdr:col>15</xdr:col>
       <xdr:colOff>254000</xdr:colOff>
       <xdr:row>52</xdr:row>
       <xdr:rowOff>169334</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>21</xdr:col>
+      <xdr:col>19</xdr:col>
       <xdr:colOff>440266</xdr:colOff>
       <xdr:row>60</xdr:row>
       <xdr:rowOff>186267</xdr:rowOff>
@@ -1695,7 +1730,7 @@
         <xdr:cNvPr id="22" name="Rectangle 21">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CCE397B4-64DA-DE46-AF5E-66940D948291}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{72001CFC-B712-6948-8A5A-5006A357B2F9}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1747,13 +1782,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
+      <xdr:col>6</xdr:col>
       <xdr:colOff>126999</xdr:colOff>
       <xdr:row>17</xdr:row>
       <xdr:rowOff>33981</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
+      <xdr:col>14</xdr:col>
       <xdr:colOff>804562</xdr:colOff>
       <xdr:row>22</xdr:row>
       <xdr:rowOff>93876</xdr:rowOff>
@@ -1763,7 +1798,7 @@
         <xdr:cNvPr id="23" name="Straight Arrow Connector 22">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E4C3C04F-6662-D948-A530-D37DE105CCC3}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{54A5899A-C307-9A4C-94DD-6EF670401A16}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1803,13 +1838,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>19</xdr:col>
+      <xdr:col>17</xdr:col>
       <xdr:colOff>347133</xdr:colOff>
       <xdr:row>40</xdr:row>
       <xdr:rowOff>72159</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>23</xdr:col>
+      <xdr:col>21</xdr:col>
       <xdr:colOff>722477</xdr:colOff>
       <xdr:row>52</xdr:row>
       <xdr:rowOff>169334</xdr:rowOff>
@@ -1819,7 +1854,7 @@
         <xdr:cNvPr id="24" name="Straight Arrow Connector 23">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{68AD627A-7079-AE42-B42A-4591DFCE4CE2}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9E1CB689-E87D-374C-B6AB-255156F33E29}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1861,25 +1896,26 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{835927DE-8815-EF46-99F7-0DF9B01410F4}" name="Table1" displayName="Table1" ref="A1:C15" totalsRowShown="0">
-  <autoFilter ref="A1:C15" xr:uid="{835927DE-8815-EF46-99F7-0DF9B01410F4}"/>
-  <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{450BF35A-9FCC-1145-8BFE-45939F271A92}" name="IDSong"/>
-    <tableColumn id="2" xr3:uid="{D5EA15CA-0A28-5F48-BB1E-6650B5FB81C2}" name="Duration(ms)"/>
-    <tableColumn id="3" xr3:uid="{82180FAF-280A-B24D-A6B4-8DCA8D912F99}" name="Frequency(Hz)" dataDxfId="6"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:D15" totalsRowShown="0">
+  <autoFilter ref="A1:D15" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="IdSong"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Duration(ms)"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Frequency(Hz)" dataDxfId="6"/>
+    <tableColumn id="4" xr3:uid="{12326ACB-010A-764E-ACFB-A808F40F5A4D}" name="Decibel(db)"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{EEC351DF-B4FF-0646-94F1-C310C8DD727D}" name="Table2" displayName="Table2" ref="A1:D2" totalsRowShown="0" headerRowDxfId="1" dataDxfId="0">
-  <autoFilter ref="A1:D2" xr:uid="{EEC351DF-B4FF-0646-94F1-C310C8DD727D}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table2" displayName="Table2" ref="A1:D2" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
+  <autoFilter ref="A1:D2" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{E99718A0-1938-684D-BEAA-C3B93C019C29}" name="IDSong" dataDxfId="5"/>
-    <tableColumn id="2" xr3:uid="{A4D5759E-75E7-5745-B428-0C5D8E3708D8}" name="Tempo" dataDxfId="4"/>
-    <tableColumn id="3" xr3:uid="{3AEF52CE-DBA3-8242-B152-38551FF06277}" name="Key" dataDxfId="3"/>
-    <tableColumn id="4" xr3:uid="{2FF6B7FC-9AA9-AD49-8A18-E41A6F579806}" name="TimeSignature" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="IdSong" dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Tempo" dataDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Key" dataDxfId="1"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="TimeSignature" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2201,31 +2237,35 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25138379-DD64-5E40-9BE1-27C8B5E1E507}">
-  <dimension ref="A1:C15"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L14" sqref="L14"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="2" max="2" width="14.6640625" customWidth="1"/>
     <col min="3" max="3" width="15.5" customWidth="1"/>
+    <col min="4" max="4" width="13.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="B1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="18">
+      <c r="D1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="18" customHeight="1">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2236,7 +2276,7 @@
         <v>261.63</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="18">
+    <row r="3" spans="1:4" ht="18" customHeight="1">
       <c r="A3">
         <v>1</v>
       </c>
@@ -2247,7 +2287,7 @@
         <v>261.63</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="18">
+    <row r="4" spans="1:4" ht="18" customHeight="1">
       <c r="A4">
         <v>1</v>
       </c>
@@ -2258,7 +2298,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="18">
+    <row r="5" spans="1:4" ht="18" customHeight="1">
       <c r="A5">
         <v>1</v>
       </c>
@@ -2269,7 +2309,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="18">
+    <row r="6" spans="1:4" ht="18" customHeight="1">
       <c r="A6">
         <v>1</v>
       </c>
@@ -2280,7 +2320,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="18">
+    <row r="7" spans="1:4" ht="18" customHeight="1">
       <c r="A7">
         <v>1</v>
       </c>
@@ -2291,7 +2331,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="18">
+    <row r="8" spans="1:4" ht="18" customHeight="1">
       <c r="A8">
         <v>1</v>
       </c>
@@ -2302,7 +2342,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="18">
+    <row r="9" spans="1:4" ht="18" customHeight="1">
       <c r="A9">
         <v>1</v>
       </c>
@@ -2313,7 +2353,7 @@
         <v>349.23</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="18">
+    <row r="10" spans="1:4" ht="18" customHeight="1">
       <c r="A10">
         <v>1</v>
       </c>
@@ -2324,7 +2364,7 @@
         <v>349.23</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="18">
+    <row r="11" spans="1:4" ht="18" customHeight="1">
       <c r="A11">
         <v>1</v>
       </c>
@@ -2335,7 +2375,7 @@
         <v>329.63</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="18">
+    <row r="12" spans="1:4" ht="18" customHeight="1">
       <c r="A12">
         <v>1</v>
       </c>
@@ -2346,7 +2386,7 @@
         <v>329.63</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="18">
+    <row r="13" spans="1:4" ht="18" customHeight="1">
       <c r="A13">
         <v>1</v>
       </c>
@@ -2357,7 +2397,7 @@
         <v>293.66000000000003</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="18">
+    <row r="14" spans="1:4" ht="18" customHeight="1">
       <c r="A14">
         <v>1</v>
       </c>
@@ -2368,7 +2408,7 @@
         <v>293.66000000000003</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="18">
+    <row r="15" spans="1:4" ht="18" customHeight="1">
       <c r="A15">
         <v>1</v>
       </c>
@@ -2381,6 +2421,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
   </tableParts>
@@ -2388,11 +2429,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19AC43FA-0314-0A45-B9FF-F9BEFE45DA2F}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -2403,16 +2444,16 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="3" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -2423,10 +2464,10 @@
         <v>60</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2" s="3">
-        <v>4</v>
+        <v>6</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -2438,42 +2479,198 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48C4D8DE-B7E4-1C4A-B099-79BFF4A8E6AA}">
-  <dimension ref="A1:C1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="A1:C1"/>
+      <selection activeCell="D1" sqref="D1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5">
+        <v>1</v>
+      </c>
+      <c r="B5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6">
+        <v>1</v>
+      </c>
+      <c r="B6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7">
+        <v>1</v>
+      </c>
+      <c r="B7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8">
+        <v>1</v>
+      </c>
+      <c r="B8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9">
+        <v>1</v>
+      </c>
+      <c r="B9" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10">
+        <v>1</v>
+      </c>
+      <c r="B10" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11">
+        <v>1</v>
+      </c>
+      <c r="B11" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12">
+        <v>1</v>
+      </c>
+      <c r="B12" t="s">
+        <v>15</v>
+      </c>
+      <c r="C12" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13">
+        <v>1</v>
+      </c>
+      <c r="B13" t="s">
+        <v>16</v>
+      </c>
+      <c r="C13" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14">
+        <v>1</v>
+      </c>
+      <c r="B14" t="s">
+        <v>16</v>
+      </c>
+      <c r="C14" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15">
+        <v>1</v>
+      </c>
+      <c r="B15" t="s">
+        <v>6</v>
+      </c>
+      <c r="C15" t="s">
+        <v>13</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <dimension ref="B4:AJ77"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection sqref="A1:AI71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A0F935EE-C919-734C-A702-9FE1EBBFF1A5}">
-  <dimension ref="D4:AJ77"/>
-  <sheetViews>
-    <sheetView topLeftCell="G10" zoomScale="89" workbookViewId="0">
-      <selection activeCell="AK54" sqref="AK54"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
-  <sheetData>
-    <row r="4" spans="4:36" ht="20">
+    <row r="4" spans="2:36" ht="20" customHeight="1">
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
@@ -2505,10 +2702,11 @@
       <c r="AF4" s="1"/>
       <c r="AG4" s="1"/>
       <c r="AH4" s="1"/>
-      <c r="AI4" s="1"/>
       <c r="AJ4" s="1"/>
     </row>
-    <row r="5" spans="4:36" ht="20">
+    <row r="5" spans="2:36" ht="20" customHeight="1">
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
@@ -2540,10 +2738,11 @@
       <c r="AF5" s="1"/>
       <c r="AG5" s="1"/>
       <c r="AH5" s="1"/>
-      <c r="AI5" s="1"/>
       <c r="AJ5" s="1"/>
     </row>
-    <row r="6" spans="4:36" ht="20">
+    <row r="6" spans="2:36" ht="20" customHeight="1">
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
@@ -2575,10 +2774,11 @@
       <c r="AF6" s="1"/>
       <c r="AG6" s="1"/>
       <c r="AH6" s="1"/>
-      <c r="AI6" s="1"/>
       <c r="AJ6" s="1"/>
     </row>
-    <row r="7" spans="4:36" ht="20">
+    <row r="7" spans="2:36" ht="20" customHeight="1">
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
@@ -2610,10 +2810,11 @@
       <c r="AF7" s="1"/>
       <c r="AG7" s="1"/>
       <c r="AH7" s="1"/>
-      <c r="AI7" s="1"/>
       <c r="AJ7" s="1"/>
     </row>
-    <row r="8" spans="4:36" ht="20">
+    <row r="8" spans="2:36" ht="20" customHeight="1">
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
@@ -2645,10 +2846,11 @@
       <c r="AF8" s="1"/>
       <c r="AG8" s="1"/>
       <c r="AH8" s="1"/>
-      <c r="AI8" s="1"/>
       <c r="AJ8" s="1"/>
     </row>
-    <row r="9" spans="4:36" ht="20">
+    <row r="9" spans="2:36" ht="20" customHeight="1">
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
@@ -2680,10 +2882,11 @@
       <c r="AF9" s="1"/>
       <c r="AG9" s="1"/>
       <c r="AH9" s="1"/>
-      <c r="AI9" s="1"/>
       <c r="AJ9" s="1"/>
     </row>
-    <row r="10" spans="4:36" ht="20">
+    <row r="10" spans="2:36" ht="20" customHeight="1">
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
@@ -2715,10 +2918,11 @@
       <c r="AF10" s="1"/>
       <c r="AG10" s="1"/>
       <c r="AH10" s="1"/>
-      <c r="AI10" s="1"/>
       <c r="AJ10" s="1"/>
     </row>
-    <row r="11" spans="4:36" ht="20">
+    <row r="11" spans="2:36" ht="20" customHeight="1">
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
@@ -2750,10 +2954,11 @@
       <c r="AF11" s="1"/>
       <c r="AG11" s="1"/>
       <c r="AH11" s="1"/>
-      <c r="AI11" s="1"/>
       <c r="AJ11" s="1"/>
     </row>
-    <row r="12" spans="4:36" ht="20">
+    <row r="12" spans="2:36" ht="20" customHeight="1">
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
@@ -2785,10 +2990,11 @@
       <c r="AF12" s="1"/>
       <c r="AG12" s="1"/>
       <c r="AH12" s="1"/>
-      <c r="AI12" s="1"/>
       <c r="AJ12" s="1"/>
     </row>
-    <row r="13" spans="4:36" ht="20">
+    <row r="13" spans="2:36" ht="20" customHeight="1">
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
@@ -2820,10 +3026,11 @@
       <c r="AF13" s="1"/>
       <c r="AG13" s="1"/>
       <c r="AH13" s="1"/>
-      <c r="AI13" s="1"/>
       <c r="AJ13" s="1"/>
     </row>
-    <row r="14" spans="4:36" ht="20">
+    <row r="14" spans="2:36" ht="20" customHeight="1">
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
@@ -2855,10 +3062,11 @@
       <c r="AF14" s="1"/>
       <c r="AG14" s="1"/>
       <c r="AH14" s="1"/>
-      <c r="AI14" s="1"/>
       <c r="AJ14" s="1"/>
     </row>
-    <row r="15" spans="4:36" ht="20">
+    <row r="15" spans="2:36" ht="20" customHeight="1">
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
@@ -2890,10 +3098,11 @@
       <c r="AF15" s="1"/>
       <c r="AG15" s="1"/>
       <c r="AH15" s="1"/>
-      <c r="AI15" s="1"/>
       <c r="AJ15" s="1"/>
     </row>
-    <row r="16" spans="4:36" ht="20">
+    <row r="16" spans="2:36" ht="20" customHeight="1">
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
@@ -2925,10 +3134,11 @@
       <c r="AF16" s="1"/>
       <c r="AG16" s="1"/>
       <c r="AH16" s="1"/>
-      <c r="AI16" s="1"/>
       <c r="AJ16" s="1"/>
     </row>
-    <row r="17" spans="4:36" ht="20">
+    <row r="17" spans="2:36" ht="20" customHeight="1">
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
@@ -2960,10 +3170,11 @@
       <c r="AF17" s="1"/>
       <c r="AG17" s="1"/>
       <c r="AH17" s="1"/>
-      <c r="AI17" s="1"/>
       <c r="AJ17" s="1"/>
     </row>
-    <row r="18" spans="4:36" ht="20">
+    <row r="18" spans="2:36" ht="20" customHeight="1">
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>
@@ -2995,10 +3206,11 @@
       <c r="AF18" s="1"/>
       <c r="AG18" s="1"/>
       <c r="AH18" s="1"/>
-      <c r="AI18" s="1"/>
       <c r="AJ18" s="1"/>
     </row>
-    <row r="19" spans="4:36" ht="20">
+    <row r="19" spans="2:36" ht="20" customHeight="1">
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
       <c r="F19" s="1"/>
@@ -3030,10 +3242,11 @@
       <c r="AF19" s="1"/>
       <c r="AG19" s="1"/>
       <c r="AH19" s="1"/>
-      <c r="AI19" s="1"/>
       <c r="AJ19" s="1"/>
     </row>
-    <row r="20" spans="4:36" ht="20">
+    <row r="20" spans="2:36" ht="20" customHeight="1">
+      <c r="B20" s="1"/>
+      <c r="C20" s="1"/>
       <c r="D20" s="1"/>
       <c r="E20" s="1"/>
       <c r="F20" s="1"/>
@@ -3065,10 +3278,11 @@
       <c r="AF20" s="1"/>
       <c r="AG20" s="1"/>
       <c r="AH20" s="1"/>
-      <c r="AI20" s="1"/>
       <c r="AJ20" s="1"/>
     </row>
-    <row r="21" spans="4:36" ht="20">
+    <row r="21" spans="2:36" ht="20" customHeight="1">
+      <c r="B21" s="1"/>
+      <c r="C21" s="1"/>
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
       <c r="F21" s="1"/>
@@ -3100,10 +3314,11 @@
       <c r="AF21" s="1"/>
       <c r="AG21" s="1"/>
       <c r="AH21" s="1"/>
-      <c r="AI21" s="1"/>
       <c r="AJ21" s="1"/>
     </row>
-    <row r="22" spans="4:36" ht="20">
+    <row r="22" spans="2:36" ht="20" customHeight="1">
+      <c r="B22" s="1"/>
+      <c r="C22" s="1"/>
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>
       <c r="F22" s="1"/>
@@ -3135,10 +3350,11 @@
       <c r="AF22" s="1"/>
       <c r="AG22" s="1"/>
       <c r="AH22" s="1"/>
-      <c r="AI22" s="1"/>
       <c r="AJ22" s="1"/>
     </row>
-    <row r="23" spans="4:36" ht="20">
+    <row r="23" spans="2:36" ht="20" customHeight="1">
+      <c r="B23" s="1"/>
+      <c r="C23" s="1"/>
       <c r="D23" s="1"/>
       <c r="E23" s="1"/>
       <c r="F23" s="1"/>
@@ -3170,10 +3386,11 @@
       <c r="AF23" s="1"/>
       <c r="AG23" s="1"/>
       <c r="AH23" s="1"/>
-      <c r="AI23" s="1"/>
       <c r="AJ23" s="1"/>
     </row>
-    <row r="24" spans="4:36" ht="20">
+    <row r="24" spans="2:36" ht="20" customHeight="1">
+      <c r="B24" s="1"/>
+      <c r="C24" s="1"/>
       <c r="D24" s="1"/>
       <c r="E24" s="1"/>
       <c r="F24" s="1"/>
@@ -3205,10 +3422,11 @@
       <c r="AF24" s="1"/>
       <c r="AG24" s="1"/>
       <c r="AH24" s="1"/>
-      <c r="AI24" s="1"/>
       <c r="AJ24" s="1"/>
     </row>
-    <row r="25" spans="4:36" ht="20">
+    <row r="25" spans="2:36" ht="20" customHeight="1">
+      <c r="B25" s="1"/>
+      <c r="C25" s="1"/>
       <c r="D25" s="1"/>
       <c r="E25" s="1"/>
       <c r="F25" s="1"/>
@@ -3240,10 +3458,11 @@
       <c r="AF25" s="1"/>
       <c r="AG25" s="1"/>
       <c r="AH25" s="1"/>
-      <c r="AI25" s="1"/>
       <c r="AJ25" s="1"/>
     </row>
-    <row r="26" spans="4:36" ht="20">
+    <row r="26" spans="2:36" ht="20" customHeight="1">
+      <c r="B26" s="1"/>
+      <c r="C26" s="1"/>
       <c r="D26" s="1"/>
       <c r="E26" s="1"/>
       <c r="F26" s="1"/>
@@ -3275,10 +3494,11 @@
       <c r="AF26" s="1"/>
       <c r="AG26" s="1"/>
       <c r="AH26" s="1"/>
-      <c r="AI26" s="1"/>
       <c r="AJ26" s="1"/>
     </row>
-    <row r="27" spans="4:36" ht="20">
+    <row r="27" spans="2:36" ht="20" customHeight="1">
+      <c r="B27" s="1"/>
+      <c r="C27" s="1"/>
       <c r="D27" s="1"/>
       <c r="E27" s="1"/>
       <c r="F27" s="1"/>
@@ -3310,10 +3530,11 @@
       <c r="AF27" s="1"/>
       <c r="AG27" s="1"/>
       <c r="AH27" s="1"/>
-      <c r="AI27" s="1"/>
       <c r="AJ27" s="1"/>
     </row>
-    <row r="28" spans="4:36" ht="20">
+    <row r="28" spans="2:36" ht="20" customHeight="1">
+      <c r="B28" s="1"/>
+      <c r="C28" s="1"/>
       <c r="D28" s="1"/>
       <c r="E28" s="1"/>
       <c r="F28" s="1"/>
@@ -3345,10 +3566,11 @@
       <c r="AF28" s="1"/>
       <c r="AG28" s="1"/>
       <c r="AH28" s="1"/>
-      <c r="AI28" s="1"/>
       <c r="AJ28" s="1"/>
     </row>
-    <row r="29" spans="4:36" ht="20">
+    <row r="29" spans="2:36" ht="20" customHeight="1">
+      <c r="B29" s="1"/>
+      <c r="C29" s="1"/>
       <c r="D29" s="1"/>
       <c r="E29" s="1"/>
       <c r="F29" s="1"/>
@@ -3380,10 +3602,11 @@
       <c r="AF29" s="1"/>
       <c r="AG29" s="1"/>
       <c r="AH29" s="1"/>
-      <c r="AI29" s="1"/>
       <c r="AJ29" s="1"/>
     </row>
-    <row r="30" spans="4:36" ht="20">
+    <row r="30" spans="2:36" ht="20" customHeight="1">
+      <c r="B30" s="1"/>
+      <c r="C30" s="1"/>
       <c r="D30" s="1"/>
       <c r="E30" s="1"/>
       <c r="F30" s="1"/>
@@ -3415,10 +3638,11 @@
       <c r="AF30" s="1"/>
       <c r="AG30" s="1"/>
       <c r="AH30" s="1"/>
-      <c r="AI30" s="1"/>
       <c r="AJ30" s="1"/>
     </row>
-    <row r="31" spans="4:36" ht="20">
+    <row r="31" spans="2:36" ht="20" customHeight="1">
+      <c r="B31" s="1"/>
+      <c r="C31" s="1"/>
       <c r="D31" s="1"/>
       <c r="E31" s="1"/>
       <c r="F31" s="1"/>
@@ -3450,10 +3674,11 @@
       <c r="AF31" s="1"/>
       <c r="AG31" s="1"/>
       <c r="AH31" s="1"/>
-      <c r="AI31" s="1"/>
       <c r="AJ31" s="1"/>
     </row>
-    <row r="32" spans="4:36" ht="20">
+    <row r="32" spans="2:36" ht="20" customHeight="1">
+      <c r="B32" s="1"/>
+      <c r="C32" s="1"/>
       <c r="D32" s="1"/>
       <c r="E32" s="1"/>
       <c r="F32" s="1"/>
@@ -3485,10 +3710,11 @@
       <c r="AF32" s="1"/>
       <c r="AG32" s="1"/>
       <c r="AH32" s="1"/>
-      <c r="AI32" s="1"/>
       <c r="AJ32" s="1"/>
     </row>
-    <row r="33" spans="4:36" ht="20">
+    <row r="33" spans="2:36" ht="20" customHeight="1">
+      <c r="B33" s="1"/>
+      <c r="C33" s="1"/>
       <c r="D33" s="1"/>
       <c r="E33" s="1"/>
       <c r="F33" s="1"/>
@@ -3520,10 +3746,11 @@
       <c r="AF33" s="1"/>
       <c r="AG33" s="1"/>
       <c r="AH33" s="1"/>
-      <c r="AI33" s="1"/>
       <c r="AJ33" s="1"/>
     </row>
-    <row r="34" spans="4:36" ht="20">
+    <row r="34" spans="2:36" ht="20" customHeight="1">
+      <c r="B34" s="1"/>
+      <c r="C34" s="1"/>
       <c r="D34" s="1"/>
       <c r="E34" s="1"/>
       <c r="F34" s="1"/>
@@ -3555,10 +3782,11 @@
       <c r="AF34" s="1"/>
       <c r="AG34" s="1"/>
       <c r="AH34" s="1"/>
-      <c r="AI34" s="1"/>
       <c r="AJ34" s="1"/>
     </row>
-    <row r="35" spans="4:36" ht="20">
+    <row r="35" spans="2:36" ht="20" customHeight="1">
+      <c r="B35" s="1"/>
+      <c r="C35" s="1"/>
       <c r="D35" s="1"/>
       <c r="E35" s="1"/>
       <c r="F35" s="1"/>
@@ -3590,10 +3818,11 @@
       <c r="AF35" s="1"/>
       <c r="AG35" s="1"/>
       <c r="AH35" s="1"/>
-      <c r="AI35" s="1"/>
       <c r="AJ35" s="1"/>
     </row>
-    <row r="36" spans="4:36" ht="20">
+    <row r="36" spans="2:36" ht="20" customHeight="1">
+      <c r="B36" s="1"/>
+      <c r="C36" s="1"/>
       <c r="D36" s="1"/>
       <c r="E36" s="1"/>
       <c r="F36" s="1"/>
@@ -3625,10 +3854,11 @@
       <c r="AF36" s="1"/>
       <c r="AG36" s="1"/>
       <c r="AH36" s="1"/>
-      <c r="AI36" s="1"/>
       <c r="AJ36" s="1"/>
     </row>
-    <row r="37" spans="4:36" ht="20">
+    <row r="37" spans="2:36" ht="20" customHeight="1">
+      <c r="B37" s="1"/>
+      <c r="C37" s="1"/>
       <c r="D37" s="1"/>
       <c r="E37" s="1"/>
       <c r="F37" s="1"/>
@@ -3660,10 +3890,11 @@
       <c r="AF37" s="1"/>
       <c r="AG37" s="1"/>
       <c r="AH37" s="1"/>
-      <c r="AI37" s="1"/>
       <c r="AJ37" s="1"/>
     </row>
-    <row r="38" spans="4:36" ht="20">
+    <row r="38" spans="2:36" ht="20" customHeight="1">
+      <c r="B38" s="1"/>
+      <c r="C38" s="1"/>
       <c r="D38" s="1"/>
       <c r="E38" s="1"/>
       <c r="F38" s="1"/>
@@ -3695,10 +3926,11 @@
       <c r="AF38" s="1"/>
       <c r="AG38" s="1"/>
       <c r="AH38" s="1"/>
-      <c r="AI38" s="1"/>
       <c r="AJ38" s="1"/>
     </row>
-    <row r="39" spans="4:36" ht="20">
+    <row r="39" spans="2:36" ht="20" customHeight="1">
+      <c r="B39" s="1"/>
+      <c r="C39" s="1"/>
       <c r="D39" s="1"/>
       <c r="E39" s="1"/>
       <c r="F39" s="1"/>
@@ -3730,10 +3962,11 @@
       <c r="AF39" s="1"/>
       <c r="AG39" s="1"/>
       <c r="AH39" s="1"/>
-      <c r="AI39" s="1"/>
       <c r="AJ39" s="1"/>
     </row>
-    <row r="40" spans="4:36" ht="20">
+    <row r="40" spans="2:36" ht="20" customHeight="1">
+      <c r="B40" s="1"/>
+      <c r="C40" s="1"/>
       <c r="D40" s="1"/>
       <c r="E40" s="1"/>
       <c r="F40" s="1"/>
@@ -3765,10 +3998,11 @@
       <c r="AF40" s="1"/>
       <c r="AG40" s="1"/>
       <c r="AH40" s="1"/>
-      <c r="AI40" s="1"/>
       <c r="AJ40" s="1"/>
     </row>
-    <row r="41" spans="4:36" ht="20">
+    <row r="41" spans="2:36" ht="20" customHeight="1">
+      <c r="B41" s="1"/>
+      <c r="C41" s="1"/>
       <c r="D41" s="1"/>
       <c r="E41" s="1"/>
       <c r="F41" s="1"/>
@@ -3800,10 +4034,11 @@
       <c r="AF41" s="1"/>
       <c r="AG41" s="1"/>
       <c r="AH41" s="1"/>
-      <c r="AI41" s="1"/>
       <c r="AJ41" s="1"/>
     </row>
-    <row r="42" spans="4:36" ht="20">
+    <row r="42" spans="2:36" ht="20" customHeight="1">
+      <c r="B42" s="1"/>
+      <c r="C42" s="1"/>
       <c r="D42" s="1"/>
       <c r="E42" s="1"/>
       <c r="F42" s="1"/>
@@ -3835,10 +4070,11 @@
       <c r="AF42" s="1"/>
       <c r="AG42" s="1"/>
       <c r="AH42" s="1"/>
-      <c r="AI42" s="1"/>
       <c r="AJ42" s="1"/>
     </row>
-    <row r="43" spans="4:36" ht="20">
+    <row r="43" spans="2:36" ht="20" customHeight="1">
+      <c r="B43" s="1"/>
+      <c r="C43" s="1"/>
       <c r="D43" s="1"/>
       <c r="E43" s="1"/>
       <c r="F43" s="1"/>
@@ -3870,10 +4106,11 @@
       <c r="AF43" s="1"/>
       <c r="AG43" s="1"/>
       <c r="AH43" s="1"/>
-      <c r="AI43" s="1"/>
       <c r="AJ43" s="1"/>
     </row>
-    <row r="44" spans="4:36" ht="20">
+    <row r="44" spans="2:36" ht="20" customHeight="1">
+      <c r="B44" s="1"/>
+      <c r="C44" s="1"/>
       <c r="D44" s="1"/>
       <c r="E44" s="1"/>
       <c r="F44" s="1"/>
@@ -3905,10 +4142,11 @@
       <c r="AF44" s="1"/>
       <c r="AG44" s="1"/>
       <c r="AH44" s="1"/>
-      <c r="AI44" s="1"/>
       <c r="AJ44" s="1"/>
     </row>
-    <row r="45" spans="4:36" ht="20">
+    <row r="45" spans="2:36" ht="20" customHeight="1">
+      <c r="B45" s="1"/>
+      <c r="C45" s="1"/>
       <c r="D45" s="1"/>
       <c r="E45" s="1"/>
       <c r="F45" s="1"/>
@@ -3940,10 +4178,11 @@
       <c r="AF45" s="1"/>
       <c r="AG45" s="1"/>
       <c r="AH45" s="1"/>
-      <c r="AI45" s="1"/>
       <c r="AJ45" s="1"/>
     </row>
-    <row r="46" spans="4:36" ht="20">
+    <row r="46" spans="2:36" ht="20" customHeight="1">
+      <c r="B46" s="1"/>
+      <c r="C46" s="1"/>
       <c r="D46" s="1"/>
       <c r="E46" s="1"/>
       <c r="F46" s="1"/>
@@ -3975,10 +4214,11 @@
       <c r="AF46" s="1"/>
       <c r="AG46" s="1"/>
       <c r="AH46" s="1"/>
-      <c r="AI46" s="1"/>
       <c r="AJ46" s="1"/>
     </row>
-    <row r="47" spans="4:36" ht="20">
+    <row r="47" spans="2:36" ht="20" customHeight="1">
+      <c r="B47" s="1"/>
+      <c r="C47" s="1"/>
       <c r="D47" s="1"/>
       <c r="E47" s="1"/>
       <c r="F47" s="1"/>
@@ -4010,10 +4250,11 @@
       <c r="AF47" s="1"/>
       <c r="AG47" s="1"/>
       <c r="AH47" s="1"/>
-      <c r="AI47" s="1"/>
       <c r="AJ47" s="1"/>
     </row>
-    <row r="48" spans="4:36" ht="20">
+    <row r="48" spans="2:36" ht="20" customHeight="1">
+      <c r="B48" s="1"/>
+      <c r="C48" s="1"/>
       <c r="D48" s="1"/>
       <c r="E48" s="1"/>
       <c r="F48" s="1"/>
@@ -4045,10 +4286,11 @@
       <c r="AF48" s="1"/>
       <c r="AG48" s="1"/>
       <c r="AH48" s="1"/>
-      <c r="AI48" s="1"/>
       <c r="AJ48" s="1"/>
     </row>
-    <row r="49" spans="4:36" ht="20">
+    <row r="49" spans="2:36" ht="20" customHeight="1">
+      <c r="B49" s="1"/>
+      <c r="C49" s="1"/>
       <c r="D49" s="1"/>
       <c r="E49" s="1"/>
       <c r="F49" s="1"/>
@@ -4080,10 +4322,11 @@
       <c r="AF49" s="1"/>
       <c r="AG49" s="1"/>
       <c r="AH49" s="1"/>
-      <c r="AI49" s="1"/>
       <c r="AJ49" s="1"/>
     </row>
-    <row r="50" spans="4:36" ht="20">
+    <row r="50" spans="2:36" ht="20" customHeight="1">
+      <c r="B50" s="1"/>
+      <c r="C50" s="1"/>
       <c r="D50" s="1"/>
       <c r="E50" s="1"/>
       <c r="F50" s="1"/>
@@ -4115,10 +4358,11 @@
       <c r="AF50" s="1"/>
       <c r="AG50" s="1"/>
       <c r="AH50" s="1"/>
-      <c r="AI50" s="1"/>
       <c r="AJ50" s="1"/>
     </row>
-    <row r="51" spans="4:36" ht="20">
+    <row r="51" spans="2:36" ht="20" customHeight="1">
+      <c r="B51" s="1"/>
+      <c r="C51" s="1"/>
       <c r="D51" s="1"/>
       <c r="E51" s="1"/>
       <c r="F51" s="1"/>
@@ -4150,10 +4394,11 @@
       <c r="AF51" s="1"/>
       <c r="AG51" s="1"/>
       <c r="AH51" s="1"/>
-      <c r="AI51" s="1"/>
       <c r="AJ51" s="1"/>
     </row>
-    <row r="52" spans="4:36" ht="20">
+    <row r="52" spans="2:36" ht="20" customHeight="1">
+      <c r="B52" s="1"/>
+      <c r="C52" s="1"/>
       <c r="D52" s="1"/>
       <c r="E52" s="1"/>
       <c r="F52" s="1"/>
@@ -4162,8 +4407,8 @@
       <c r="I52" s="1"/>
       <c r="J52" s="1"/>
       <c r="K52" s="1"/>
-      <c r="L52" s="1"/>
       <c r="M52" s="1"/>
+      <c r="N52" s="1"/>
       <c r="O52" s="1"/>
       <c r="P52" s="1"/>
       <c r="Q52" s="1"/>
@@ -4184,10 +4429,11 @@
       <c r="AF52" s="1"/>
       <c r="AG52" s="1"/>
       <c r="AH52" s="1"/>
-      <c r="AI52" s="1"/>
       <c r="AJ52" s="1"/>
     </row>
-    <row r="53" spans="4:36" ht="20">
+    <row r="53" spans="2:36" ht="20" customHeight="1">
+      <c r="B53" s="1"/>
+      <c r="C53" s="1"/>
       <c r="D53" s="1"/>
       <c r="E53" s="1"/>
       <c r="F53" s="1"/>
@@ -4196,8 +4442,8 @@
       <c r="I53" s="1"/>
       <c r="J53" s="1"/>
       <c r="K53" s="1"/>
-      <c r="L53" s="1"/>
       <c r="M53" s="1"/>
+      <c r="N53" s="1"/>
       <c r="O53" s="1"/>
       <c r="P53" s="1"/>
       <c r="Q53" s="1"/>
@@ -4218,10 +4464,11 @@
       <c r="AF53" s="1"/>
       <c r="AG53" s="1"/>
       <c r="AH53" s="1"/>
-      <c r="AI53" s="1"/>
       <c r="AJ53" s="1"/>
     </row>
-    <row r="54" spans="4:36" ht="20">
+    <row r="54" spans="2:36" ht="20" customHeight="1">
+      <c r="B54" s="1"/>
+      <c r="C54" s="1"/>
       <c r="D54" s="1"/>
       <c r="E54" s="1"/>
       <c r="F54" s="1"/>
@@ -4230,8 +4477,8 @@
       <c r="I54" s="1"/>
       <c r="J54" s="1"/>
       <c r="K54" s="1"/>
-      <c r="L54" s="1"/>
       <c r="M54" s="1"/>
+      <c r="N54" s="1"/>
       <c r="O54" s="1"/>
       <c r="P54" s="1"/>
       <c r="Q54" s="1"/>
@@ -4252,10 +4499,11 @@
       <c r="AF54" s="1"/>
       <c r="AG54" s="1"/>
       <c r="AH54" s="1"/>
-      <c r="AI54" s="1"/>
       <c r="AJ54" s="1"/>
     </row>
-    <row r="55" spans="4:36" ht="20">
+    <row r="55" spans="2:36" ht="20" customHeight="1">
+      <c r="B55" s="1"/>
+      <c r="C55" s="1"/>
       <c r="D55" s="1"/>
       <c r="E55" s="1"/>
       <c r="F55" s="1"/>
@@ -4264,8 +4512,8 @@
       <c r="I55" s="1"/>
       <c r="J55" s="1"/>
       <c r="K55" s="1"/>
-      <c r="L55" s="1"/>
       <c r="M55" s="1"/>
+      <c r="N55" s="1"/>
       <c r="O55" s="1"/>
       <c r="P55" s="1"/>
       <c r="Q55" s="1"/>
@@ -4286,10 +4534,11 @@
       <c r="AF55" s="1"/>
       <c r="AG55" s="1"/>
       <c r="AH55" s="1"/>
-      <c r="AI55" s="1"/>
       <c r="AJ55" s="1"/>
     </row>
-    <row r="56" spans="4:36" ht="20">
+    <row r="56" spans="2:36" ht="20" customHeight="1">
+      <c r="B56" s="1"/>
+      <c r="C56" s="1"/>
       <c r="D56" s="1"/>
       <c r="E56" s="1"/>
       <c r="F56" s="1"/>
@@ -4298,8 +4547,8 @@
       <c r="I56" s="1"/>
       <c r="J56" s="1"/>
       <c r="K56" s="1"/>
-      <c r="L56" s="1"/>
       <c r="M56" s="1"/>
+      <c r="N56" s="1"/>
       <c r="O56" s="1"/>
       <c r="P56" s="1"/>
       <c r="Q56" s="1"/>
@@ -4320,10 +4569,11 @@
       <c r="AF56" s="1"/>
       <c r="AG56" s="1"/>
       <c r="AH56" s="1"/>
-      <c r="AI56" s="1"/>
       <c r="AJ56" s="1"/>
     </row>
-    <row r="57" spans="4:36" ht="20">
+    <row r="57" spans="2:36" ht="20" customHeight="1">
+      <c r="B57" s="1"/>
+      <c r="C57" s="1"/>
       <c r="D57" s="1"/>
       <c r="E57" s="1"/>
       <c r="F57" s="1"/>
@@ -4332,8 +4582,8 @@
       <c r="I57" s="1"/>
       <c r="J57" s="1"/>
       <c r="K57" s="1"/>
-      <c r="L57" s="1"/>
       <c r="M57" s="1"/>
+      <c r="N57" s="1"/>
       <c r="O57" s="1"/>
       <c r="P57" s="1"/>
       <c r="Q57" s="1"/>
@@ -4354,10 +4604,11 @@
       <c r="AF57" s="1"/>
       <c r="AG57" s="1"/>
       <c r="AH57" s="1"/>
-      <c r="AI57" s="1"/>
       <c r="AJ57" s="1"/>
     </row>
-    <row r="58" spans="4:36" ht="20">
+    <row r="58" spans="2:36" ht="20" customHeight="1">
+      <c r="B58" s="1"/>
+      <c r="C58" s="1"/>
       <c r="D58" s="1"/>
       <c r="E58" s="1"/>
       <c r="F58" s="1"/>
@@ -4366,8 +4617,8 @@
       <c r="I58" s="1"/>
       <c r="J58" s="1"/>
       <c r="K58" s="1"/>
-      <c r="L58" s="1"/>
       <c r="M58" s="1"/>
+      <c r="N58" s="1"/>
       <c r="O58" s="1"/>
       <c r="P58" s="1"/>
       <c r="Q58" s="1"/>
@@ -4388,10 +4639,11 @@
       <c r="AF58" s="1"/>
       <c r="AG58" s="1"/>
       <c r="AH58" s="1"/>
-      <c r="AI58" s="1"/>
       <c r="AJ58" s="1"/>
     </row>
-    <row r="59" spans="4:36" ht="20">
+    <row r="59" spans="2:36" ht="20" customHeight="1">
+      <c r="B59" s="1"/>
+      <c r="C59" s="1"/>
       <c r="D59" s="1"/>
       <c r="E59" s="1"/>
       <c r="F59" s="1"/>
@@ -4400,8 +4652,8 @@
       <c r="I59" s="1"/>
       <c r="J59" s="1"/>
       <c r="K59" s="1"/>
-      <c r="L59" s="1"/>
       <c r="M59" s="1"/>
+      <c r="N59" s="1"/>
       <c r="O59" s="1"/>
       <c r="P59" s="1"/>
       <c r="Q59" s="1"/>
@@ -4422,10 +4674,11 @@
       <c r="AF59" s="1"/>
       <c r="AG59" s="1"/>
       <c r="AH59" s="1"/>
-      <c r="AI59" s="1"/>
       <c r="AJ59" s="1"/>
     </row>
-    <row r="60" spans="4:36" ht="20">
+    <row r="60" spans="2:36" ht="20" customHeight="1">
+      <c r="B60" s="1"/>
+      <c r="C60" s="1"/>
       <c r="D60" s="1"/>
       <c r="E60" s="1"/>
       <c r="F60" s="1"/>
@@ -4434,8 +4687,8 @@
       <c r="I60" s="1"/>
       <c r="J60" s="1"/>
       <c r="K60" s="1"/>
-      <c r="L60" s="1"/>
       <c r="M60" s="1"/>
+      <c r="N60" s="1"/>
       <c r="O60" s="1"/>
       <c r="P60" s="1"/>
       <c r="Q60" s="1"/>
@@ -4456,10 +4709,11 @@
       <c r="AF60" s="1"/>
       <c r="AG60" s="1"/>
       <c r="AH60" s="1"/>
-      <c r="AI60" s="1"/>
       <c r="AJ60" s="1"/>
     </row>
-    <row r="61" spans="4:36" ht="20">
+    <row r="61" spans="2:36" ht="20" customHeight="1">
+      <c r="B61" s="1"/>
+      <c r="C61" s="1"/>
       <c r="D61" s="1"/>
       <c r="E61" s="1"/>
       <c r="F61" s="1"/>
@@ -4468,8 +4722,8 @@
       <c r="I61" s="1"/>
       <c r="J61" s="1"/>
       <c r="K61" s="1"/>
-      <c r="L61" s="1"/>
       <c r="M61" s="1"/>
+      <c r="N61" s="1"/>
       <c r="O61" s="1"/>
       <c r="P61" s="1"/>
       <c r="Q61" s="1"/>
@@ -4490,10 +4744,11 @@
       <c r="AF61" s="1"/>
       <c r="AG61" s="1"/>
       <c r="AH61" s="1"/>
-      <c r="AI61" s="1"/>
       <c r="AJ61" s="1"/>
     </row>
-    <row r="62" spans="4:36" ht="20">
+    <row r="62" spans="2:36" ht="20" customHeight="1">
+      <c r="B62" s="1"/>
+      <c r="C62" s="1"/>
       <c r="D62" s="1"/>
       <c r="E62" s="1"/>
       <c r="F62" s="1"/>
@@ -4502,8 +4757,8 @@
       <c r="I62" s="1"/>
       <c r="J62" s="1"/>
       <c r="K62" s="1"/>
-      <c r="L62" s="1"/>
       <c r="M62" s="1"/>
+      <c r="N62" s="1"/>
       <c r="O62" s="1"/>
       <c r="P62" s="1"/>
       <c r="Q62" s="1"/>
@@ -4524,10 +4779,11 @@
       <c r="AF62" s="1"/>
       <c r="AG62" s="1"/>
       <c r="AH62" s="1"/>
-      <c r="AI62" s="1"/>
       <c r="AJ62" s="1"/>
     </row>
-    <row r="63" spans="4:36" ht="20">
+    <row r="63" spans="2:36" ht="20" customHeight="1">
+      <c r="B63" s="1"/>
+      <c r="C63" s="1"/>
       <c r="D63" s="1"/>
       <c r="E63" s="1"/>
       <c r="F63" s="1"/>
@@ -4536,8 +4792,8 @@
       <c r="I63" s="1"/>
       <c r="J63" s="1"/>
       <c r="K63" s="1"/>
-      <c r="L63" s="1"/>
       <c r="M63" s="1"/>
+      <c r="N63" s="1"/>
       <c r="O63" s="1"/>
       <c r="P63" s="1"/>
       <c r="Q63" s="1"/>
@@ -4558,10 +4814,11 @@
       <c r="AF63" s="1"/>
       <c r="AG63" s="1"/>
       <c r="AH63" s="1"/>
-      <c r="AI63" s="1"/>
       <c r="AJ63" s="1"/>
     </row>
-    <row r="64" spans="4:36" ht="20">
+    <row r="64" spans="2:36" ht="20" customHeight="1">
+      <c r="B64" s="1"/>
+      <c r="C64" s="1"/>
       <c r="D64" s="1"/>
       <c r="E64" s="1"/>
       <c r="F64" s="1"/>
@@ -4570,8 +4827,8 @@
       <c r="I64" s="1"/>
       <c r="J64" s="1"/>
       <c r="K64" s="1"/>
-      <c r="L64" s="1"/>
       <c r="M64" s="1"/>
+      <c r="N64" s="1"/>
       <c r="O64" s="1"/>
       <c r="P64" s="1"/>
       <c r="Q64" s="1"/>
@@ -4592,10 +4849,11 @@
       <c r="AF64" s="1"/>
       <c r="AG64" s="1"/>
       <c r="AH64" s="1"/>
-      <c r="AI64" s="1"/>
       <c r="AJ64" s="1"/>
     </row>
-    <row r="65" spans="4:36" ht="20">
+    <row r="65" spans="2:36" ht="20" customHeight="1">
+      <c r="B65" s="1"/>
+      <c r="C65" s="1"/>
       <c r="D65" s="1"/>
       <c r="E65" s="1"/>
       <c r="F65" s="1"/>
@@ -4604,8 +4862,8 @@
       <c r="I65" s="1"/>
       <c r="J65" s="1"/>
       <c r="K65" s="1"/>
-      <c r="L65" s="1"/>
       <c r="M65" s="1"/>
+      <c r="N65" s="1"/>
       <c r="O65" s="1"/>
       <c r="P65" s="1"/>
       <c r="Q65" s="1"/>
@@ -4626,10 +4884,11 @@
       <c r="AF65" s="1"/>
       <c r="AG65" s="1"/>
       <c r="AH65" s="1"/>
-      <c r="AI65" s="1"/>
       <c r="AJ65" s="1"/>
     </row>
-    <row r="66" spans="4:36" ht="20">
+    <row r="66" spans="2:36" ht="20" customHeight="1">
+      <c r="B66" s="1"/>
+      <c r="C66" s="1"/>
       <c r="D66" s="1"/>
       <c r="E66" s="1"/>
       <c r="F66" s="1"/>
@@ -4638,8 +4897,8 @@
       <c r="I66" s="1"/>
       <c r="J66" s="1"/>
       <c r="K66" s="1"/>
-      <c r="L66" s="1"/>
       <c r="M66" s="1"/>
+      <c r="N66" s="1"/>
       <c r="O66" s="1"/>
       <c r="P66" s="1"/>
       <c r="Q66" s="1"/>
@@ -4660,10 +4919,11 @@
       <c r="AF66" s="1"/>
       <c r="AG66" s="1"/>
       <c r="AH66" s="1"/>
-      <c r="AI66" s="1"/>
       <c r="AJ66" s="1"/>
     </row>
-    <row r="67" spans="4:36" ht="20">
+    <row r="67" spans="2:36" ht="20" customHeight="1">
+      <c r="B67" s="1"/>
+      <c r="C67" s="1"/>
       <c r="D67" s="1"/>
       <c r="E67" s="1"/>
       <c r="F67" s="1"/>
@@ -4672,8 +4932,8 @@
       <c r="I67" s="1"/>
       <c r="J67" s="1"/>
       <c r="K67" s="1"/>
-      <c r="L67" s="1"/>
       <c r="M67" s="1"/>
+      <c r="N67" s="1"/>
       <c r="O67" s="1"/>
       <c r="P67" s="1"/>
       <c r="Q67" s="1"/>
@@ -4694,10 +4954,11 @@
       <c r="AF67" s="1"/>
       <c r="AG67" s="1"/>
       <c r="AH67" s="1"/>
-      <c r="AI67" s="1"/>
       <c r="AJ67" s="1"/>
     </row>
-    <row r="68" spans="4:36" ht="20">
+    <row r="68" spans="2:36" ht="20" customHeight="1">
+      <c r="B68" s="1"/>
+      <c r="C68" s="1"/>
       <c r="D68" s="1"/>
       <c r="E68" s="1"/>
       <c r="F68" s="1"/>
@@ -4706,8 +4967,8 @@
       <c r="I68" s="1"/>
       <c r="J68" s="1"/>
       <c r="K68" s="1"/>
-      <c r="L68" s="1"/>
       <c r="M68" s="1"/>
+      <c r="N68" s="1"/>
       <c r="O68" s="1"/>
       <c r="P68" s="1"/>
       <c r="Q68" s="1"/>
@@ -4728,10 +4989,11 @@
       <c r="AF68" s="1"/>
       <c r="AG68" s="1"/>
       <c r="AH68" s="1"/>
-      <c r="AI68" s="1"/>
       <c r="AJ68" s="1"/>
     </row>
-    <row r="69" spans="4:36" ht="20">
+    <row r="69" spans="2:36" ht="20" customHeight="1">
+      <c r="B69" s="1"/>
+      <c r="C69" s="1"/>
       <c r="D69" s="1"/>
       <c r="E69" s="1"/>
       <c r="F69" s="1"/>
@@ -4740,8 +5002,8 @@
       <c r="I69" s="1"/>
       <c r="J69" s="1"/>
       <c r="K69" s="1"/>
-      <c r="L69" s="1"/>
       <c r="M69" s="1"/>
+      <c r="N69" s="1"/>
       <c r="O69" s="1"/>
       <c r="P69" s="1"/>
       <c r="Q69" s="1"/>
@@ -4762,10 +5024,11 @@
       <c r="AF69" s="1"/>
       <c r="AG69" s="1"/>
       <c r="AH69" s="1"/>
-      <c r="AI69" s="1"/>
       <c r="AJ69" s="1"/>
     </row>
-    <row r="70" spans="4:36" ht="20">
+    <row r="70" spans="2:36" ht="20" customHeight="1">
+      <c r="B70" s="1"/>
+      <c r="C70" s="1"/>
       <c r="D70" s="1"/>
       <c r="E70" s="1"/>
       <c r="F70" s="1"/>
@@ -4774,8 +5037,8 @@
       <c r="I70" s="1"/>
       <c r="J70" s="1"/>
       <c r="K70" s="1"/>
-      <c r="L70" s="1"/>
-      <c r="M70" s="1"/>
+      <c r="W70" s="1"/>
+      <c r="X70" s="1"/>
       <c r="Y70" s="1"/>
       <c r="Z70" s="1"/>
       <c r="AA70" s="1"/>
@@ -4786,10 +5049,11 @@
       <c r="AF70" s="1"/>
       <c r="AG70" s="1"/>
       <c r="AH70" s="1"/>
-      <c r="AI70" s="1"/>
       <c r="AJ70" s="1"/>
     </row>
-    <row r="71" spans="4:36" ht="20">
+    <row r="71" spans="2:36" ht="20" customHeight="1">
+      <c r="B71" s="1"/>
+      <c r="C71" s="1"/>
       <c r="D71" s="1"/>
       <c r="E71" s="1"/>
       <c r="F71" s="1"/>
@@ -4798,8 +5062,8 @@
       <c r="I71" s="1"/>
       <c r="J71" s="1"/>
       <c r="K71" s="1"/>
-      <c r="L71" s="1"/>
-      <c r="M71" s="1"/>
+      <c r="W71" s="1"/>
+      <c r="X71" s="1"/>
       <c r="Y71" s="1"/>
       <c r="Z71" s="1"/>
       <c r="AA71" s="1"/>
@@ -4810,10 +5074,9 @@
       <c r="AF71" s="1"/>
       <c r="AG71" s="1"/>
       <c r="AH71" s="1"/>
-      <c r="AI71" s="1"/>
       <c r="AJ71" s="1"/>
     </row>
-    <row r="72" spans="4:36" ht="20">
+    <row r="72" spans="2:36" ht="20" customHeight="1">
       <c r="D72" s="1"/>
       <c r="E72" s="1"/>
       <c r="F72" s="1"/>
@@ -4837,7 +5100,7 @@
       <c r="AI72" s="1"/>
       <c r="AJ72" s="1"/>
     </row>
-    <row r="73" spans="4:36" ht="20">
+    <row r="73" spans="2:36" ht="20" customHeight="1">
       <c r="D73" s="1"/>
       <c r="E73" s="1"/>
       <c r="F73" s="1"/>
@@ -4861,7 +5124,7 @@
       <c r="AI73" s="1"/>
       <c r="AJ73" s="1"/>
     </row>
-    <row r="74" spans="4:36" ht="20">
+    <row r="74" spans="2:36" ht="20" customHeight="1">
       <c r="D74" s="1"/>
       <c r="E74" s="1"/>
       <c r="F74" s="1"/>
@@ -4885,7 +5148,7 @@
       <c r="AI74" s="1"/>
       <c r="AJ74" s="1"/>
     </row>
-    <row r="75" spans="4:36" ht="20">
+    <row r="75" spans="2:36" ht="20" customHeight="1">
       <c r="D75" s="1"/>
       <c r="E75" s="1"/>
       <c r="F75" s="1"/>
@@ -4909,7 +5172,7 @@
       <c r="AI75" s="1"/>
       <c r="AJ75" s="1"/>
     </row>
-    <row r="76" spans="4:36" ht="20">
+    <row r="76" spans="2:36" ht="20" customHeight="1">
       <c r="D76" s="1"/>
       <c r="E76" s="1"/>
       <c r="F76" s="1"/>
@@ -4944,7 +5207,7 @@
       <c r="AI76" s="1"/>
       <c r="AJ76" s="1"/>
     </row>
-    <row r="77" spans="4:36" ht="20">
+    <row r="77" spans="2:36" ht="20" customHeight="1">
       <c r="D77" s="1"/>
       <c r="E77" s="1"/>
       <c r="F77" s="1"/>
@@ -4983,4 +5246,18 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E173E429-BAC4-BC46-8608-BD6C116A9275}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I32" sqref="I32"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>